<commit_message>
Removed MRM output files from output folder
Saved MTOM deterministic model test runs in for both July and Aug in appropriate folder
Completed excel comparison documents for deterministic model runs vs 24 MS
Moved MRM output for MTOM test runs for both July and Aug into appropriate folder

Replaced July ensemble output passthrough sheet with august to be able to complete the August MTOM test runs
</commit_message>
<xml_diff>
--- a/RW Files/TestModelRuns/08_August Models/Aug24MS_OpVsDev_MOST.xlsx
+++ b/RW Files/TestModelRuns/08_August Models/Aug24MS_OpVsDev_MOST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apivarnik\Desktop\GIT\MTOM\RW Files\TestModelRuns\08_August Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997D80FE-DE2A-4157-AE05-E0D7A82BE8BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C74852-D618-4DDB-B240-04982DA1F45B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{ACA32295-86C6-4435-AED7-5BA48188675B}"/>
   </bookViews>
@@ -290,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -307,7 +307,6 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -6135,7 +6134,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6289,80 +6288,80 @@
         <v>44</v>
       </c>
       <c r="C3" s="8">
-        <f>Monthly_Op!C3-Monthly_Op!C3</f>
-        <v>0</v>
+        <f>Monthly_Op!C3-Monthly_Dev!C3</f>
+        <v>2.5902409106492996E-9</v>
       </c>
       <c r="D3" s="8">
-        <f>Monthly_Op!D3-Monthly_Op!D3</f>
-        <v>0</v>
+        <f>Monthly_Op!D3-Monthly_Dev!D3</f>
+        <v>-2.9262063037549524E-5</v>
       </c>
       <c r="E3" s="8">
-        <f>Monthly_Op!E3-Monthly_Op!E3</f>
-        <v>0</v>
+        <f>Monthly_Op!E3-Monthly_Dev!E3</f>
+        <v>-1.6359727965209458E-5</v>
       </c>
       <c r="F3" s="8">
-        <f>Monthly_Op!F3-Monthly_Op!F3</f>
+        <f>Monthly_Op!F3-Monthly_Dev!F3</f>
         <v>0</v>
       </c>
       <c r="G3" s="8">
-        <f>Monthly_Op!G3-Monthly_Op!G3</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="10">
-        <f>Monthly_Op!H3-Monthly_Op!H3</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="10">
-        <f>Monthly_Op!I3-Monthly_Op!I3</f>
-        <v>0</v>
+        <f>Monthly_Op!G3-Monthly_Dev!G3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
+        <f>Monthly_Op!H3-Monthly_Dev!H3</f>
+        <v>-4.9208738005290797E-4</v>
+      </c>
+      <c r="I3" s="8">
+        <f>Monthly_Op!I3-Monthly_Dev!I3</f>
+        <v>4.1039976370882414E-4</v>
       </c>
       <c r="J3" s="8">
-        <f>Monthly_Op!J3-Monthly_Op!J3</f>
-        <v>0</v>
+        <f>Monthly_Op!J3-Monthly_Dev!J3</f>
+        <v>-1.220001877300092E-11</v>
       </c>
       <c r="K3" s="8">
-        <f>Monthly_Op!K3-Monthly_Op!K3</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="10">
-        <f>Monthly_Op!L3-Monthly_Op!L3</f>
-        <v>0</v>
+        <f>Monthly_Op!K3-Monthly_Dev!K3</f>
+        <v>-7.1003114499035291E-10</v>
+      </c>
+      <c r="L3" s="8">
+        <f>Monthly_Op!L3-Monthly_Dev!L3</f>
+        <v>-4.9999870989267947E-3</v>
       </c>
       <c r="M3" s="8">
-        <f>Monthly_Op!M3-Monthly_Op!M3</f>
+        <f>Monthly_Op!M3-Monthly_Dev!M3</f>
         <v>0</v>
       </c>
       <c r="N3" s="8">
-        <f>Monthly_Op!N3-Monthly_Op!N3</f>
-        <v>0</v>
+        <f>Monthly_Op!N3-Monthly_Dev!N3</f>
+        <v>-1.5039859135868028E-8</v>
       </c>
       <c r="O3" s="8">
-        <f>Monthly_Op!O3-Monthly_Op!O3</f>
-        <v>0</v>
+        <f>Monthly_Op!O3-Monthly_Dev!O3</f>
+        <v>4.3996806198265404E-10</v>
       </c>
       <c r="P3" s="8">
-        <f>Monthly_Op!P3-Monthly_Op!P3</f>
-        <v>0</v>
+        <f>Monthly_Op!P3-Monthly_Dev!P3</f>
+        <v>1.2900272849947214E-8</v>
       </c>
       <c r="Q3" s="8">
-        <f>Monthly_Op!Q3-Monthly_Op!Q3</f>
-        <v>0</v>
+        <f>Monthly_Op!Q3-Monthly_Dev!Q3</f>
+        <v>2.7339090593159199E-5</v>
       </c>
       <c r="R3" s="8">
-        <f>Monthly_Op!R3-Monthly_Op!R3</f>
-        <v>0</v>
+        <f>Monthly_Op!R3-Monthly_Dev!R3</f>
+        <v>-7.0096575655043125E-8</v>
       </c>
       <c r="S3" s="8">
-        <f>Monthly_Op!S3-Monthly_Op!S3</f>
-        <v>0</v>
+        <f>Monthly_Op!S3-Monthly_Dev!S3</f>
+        <v>-8.9203240349888802E-8</v>
       </c>
       <c r="T3" s="8">
-        <f>Monthly_Op!T3-Monthly_Op!T3</f>
-        <v>0</v>
+        <f>Monthly_Op!T3-Monthly_Dev!T3</f>
+        <v>-1.5301338862627745E-8</v>
       </c>
       <c r="U3" s="8">
-        <f>Monthly_Op!U3-Monthly_Op!U3</f>
-        <v>0</v>
+        <f>Monthly_Op!U3-Monthly_Dev!U3</f>
+        <v>-6.600748747587204E-8</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -6373,80 +6372,80 @@
         <v>45</v>
       </c>
       <c r="C4" s="8">
-        <f>Monthly_Op!C4-Monthly_Op!C4</f>
-        <v>0</v>
+        <f>Monthly_Op!C4-Monthly_Dev!C4</f>
+        <v>2.6202542358078063E-9</v>
       </c>
       <c r="D4" s="8">
-        <f>Monthly_Op!D4-Monthly_Op!D4</f>
-        <v>0</v>
+        <f>Monthly_Op!D4-Monthly_Dev!D4</f>
+        <v>-1.054985099813166E-4</v>
       </c>
       <c r="E4" s="8">
-        <f>Monthly_Op!E4-Monthly_Op!E4</f>
-        <v>0</v>
+        <f>Monthly_Op!E4-Monthly_Dev!E4</f>
+        <v>-1.6329459981534455E-5</v>
       </c>
       <c r="F4" s="8">
-        <f>Monthly_Op!F4-Monthly_Op!F4</f>
+        <f>Monthly_Op!F4-Monthly_Dev!F4</f>
         <v>0</v>
       </c>
       <c r="G4" s="8">
-        <f>Monthly_Op!G4-Monthly_Op!G4</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="10">
-        <f>Monthly_Op!H4-Monthly_Op!H4</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="10">
-        <f>Monthly_Op!I4-Monthly_Op!I4</f>
-        <v>0</v>
+        <f>Monthly_Op!G4-Monthly_Dev!G4</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <f>Monthly_Op!H4-Monthly_Dev!H4</f>
+        <v>-4.9160624985233881E-4</v>
+      </c>
+      <c r="I4" s="8">
+        <f>Monthly_Op!I4-Monthly_Dev!I4</f>
+        <v>4.103997886062416E-4</v>
       </c>
       <c r="J4" s="8">
-        <f>Monthly_Op!J4-Monthly_Op!J4</f>
-        <v>0</v>
+        <f>Monthly_Op!J4-Monthly_Dev!J4</f>
+        <v>1.5496937066927785E-11</v>
       </c>
       <c r="K4" s="8">
-        <f>Monthly_Op!K4-Monthly_Op!K4</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="10">
-        <f>Monthly_Op!L4-Monthly_Op!L4</f>
-        <v>0</v>
+        <f>Monthly_Op!K4-Monthly_Dev!K4</f>
+        <v>2.4999735614983365E-10</v>
+      </c>
+      <c r="L4" s="8">
+        <f>Monthly_Op!L4-Monthly_Dev!L4</f>
+        <v>-4.9999873008346185E-3</v>
       </c>
       <c r="M4" s="8">
-        <f>Monthly_Op!M4-Monthly_Op!M4</f>
+        <f>Monthly_Op!M4-Monthly_Dev!M4</f>
         <v>0</v>
       </c>
       <c r="N4" s="8">
-        <f>Monthly_Op!N4-Monthly_Op!N4</f>
-        <v>0</v>
+        <f>Monthly_Op!N4-Monthly_Dev!N4</f>
+        <v>-7.6988726505078375E-10</v>
       </c>
       <c r="O4" s="8">
-        <f>Monthly_Op!O4-Monthly_Op!O4</f>
-        <v>0</v>
+        <f>Monthly_Op!O4-Monthly_Dev!O4</f>
+        <v>-1.409944161423482E-9</v>
       </c>
       <c r="P4" s="8">
-        <f>Monthly_Op!P4-Monthly_Op!P4</f>
-        <v>0</v>
+        <f>Monthly_Op!P4-Monthly_Dev!P4</f>
+        <v>1.5299519873224199E-8</v>
       </c>
       <c r="Q4" s="8">
-        <f>Monthly_Op!Q4-Monthly_Op!Q4</f>
-        <v>0</v>
+        <f>Monthly_Op!Q4-Monthly_Dev!Q4</f>
+        <v>-2.7022906579077244E-5</v>
       </c>
       <c r="R4" s="8">
-        <f>Monthly_Op!R4-Monthly_Op!R4</f>
+        <f>Monthly_Op!R4-Monthly_Dev!R4</f>
         <v>0</v>
       </c>
       <c r="S4" s="8">
-        <f>Monthly_Op!S4-Monthly_Op!S4</f>
-        <v>0</v>
+        <f>Monthly_Op!S4-Monthly_Dev!S4</f>
+        <v>7.6193828135728836E-8</v>
       </c>
       <c r="T4" s="8">
-        <f>Monthly_Op!T4-Monthly_Op!T4</f>
-        <v>0</v>
+        <f>Monthly_Op!T4-Monthly_Dev!T4</f>
+        <v>-9.7999873105436563E-8</v>
       </c>
       <c r="U4" s="8">
-        <f>Monthly_Op!U4-Monthly_Op!U4</f>
-        <v>0</v>
+        <f>Monthly_Op!U4-Monthly_Dev!U4</f>
+        <v>-7.2992406785488129E-8</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -6457,80 +6456,80 @@
         <v>2</v>
       </c>
       <c r="C5" s="8">
-        <f>Monthly_Op!C5-Monthly_Op!C5</f>
-        <v>0</v>
+        <f>Monthly_Op!C5-Monthly_Dev!C5</f>
+        <v>1.2501004675868899E-9</v>
       </c>
       <c r="D5" s="8">
-        <f>Monthly_Op!D5-Monthly_Op!D5</f>
-        <v>0</v>
+        <f>Monthly_Op!D5-Monthly_Dev!D5</f>
+        <v>-1.512378030383843E-4</v>
       </c>
       <c r="E5" s="8">
-        <f>Monthly_Op!E5-Monthly_Op!E5</f>
-        <v>0</v>
+        <f>Monthly_Op!E5-Monthly_Dev!E5</f>
+        <v>-1.6372876984860341E-5</v>
       </c>
       <c r="F5" s="8">
-        <f>Monthly_Op!F5-Monthly_Op!F5</f>
+        <f>Monthly_Op!F5-Monthly_Dev!F5</f>
         <v>0</v>
       </c>
       <c r="G5" s="8">
-        <f>Monthly_Op!G5-Monthly_Op!G5</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="10">
-        <f>Monthly_Op!H5-Monthly_Op!H5</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="10">
-        <f>Monthly_Op!I5-Monthly_Op!I5</f>
-        <v>0</v>
+        <f>Monthly_Op!G5-Monthly_Dev!G5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
+        <f>Monthly_Op!H5-Monthly_Dev!H5</f>
+        <v>-4.9140596001961967E-4</v>
+      </c>
+      <c r="I5" s="8">
+        <f>Monthly_Op!I5-Monthly_Dev!I5</f>
+        <v>4.1039977550383355E-4</v>
       </c>
       <c r="J5" s="8">
-        <f>Monthly_Op!J5-Monthly_Op!J5</f>
-        <v>0</v>
+        <f>Monthly_Op!J5-Monthly_Dev!J5</f>
+        <v>-2.2701840407535201E-11</v>
       </c>
       <c r="K5" s="8">
-        <f>Monthly_Op!K5-Monthly_Op!K5</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="10">
-        <f>Monthly_Op!L5-Monthly_Op!L5</f>
-        <v>0</v>
+        <f>Monthly_Op!K5-Monthly_Dev!K5</f>
+        <v>5.999822860758286E-10</v>
+      </c>
+      <c r="L5" s="8">
+        <f>Monthly_Op!L5-Monthly_Dev!L5</f>
+        <v>-4.9999600996670779E-3</v>
       </c>
       <c r="M5" s="8">
-        <f>Monthly_Op!M5-Monthly_Op!M5</f>
+        <f>Monthly_Op!M5-Monthly_Dev!M5</f>
         <v>0</v>
       </c>
       <c r="N5" s="8">
-        <f>Monthly_Op!N5-Monthly_Op!N5</f>
-        <v>0</v>
+        <f>Monthly_Op!N5-Monthly_Dev!N5</f>
+        <v>1.1690190149238333E-8</v>
       </c>
       <c r="O5" s="8">
-        <f>Monthly_Op!O5-Monthly_Op!O5</f>
-        <v>0</v>
+        <f>Monthly_Op!O5-Monthly_Dev!O5</f>
+        <v>-4.5997694542165846E-10</v>
       </c>
       <c r="P5" s="8">
-        <f>Monthly_Op!P5-Monthly_Op!P5</f>
-        <v>0</v>
+        <f>Monthly_Op!P5-Monthly_Dev!P5</f>
+        <v>-6.2500475905835629E-8</v>
       </c>
       <c r="Q5" s="8">
-        <f>Monthly_Op!Q5-Monthly_Op!Q5</f>
-        <v>0</v>
+        <f>Monthly_Op!Q5-Monthly_Dev!Q5</f>
+        <v>2.4295062758028507E-5</v>
       </c>
       <c r="R5" s="8">
-        <f>Monthly_Op!R5-Monthly_Op!R5</f>
-        <v>0</v>
+        <f>Monthly_Op!R5-Monthly_Dev!R5</f>
+        <v>-7.0140231400728226E-9</v>
       </c>
       <c r="S5" s="8">
-        <f>Monthly_Op!S5-Monthly_Op!S5</f>
-        <v>0</v>
+        <f>Monthly_Op!S5-Monthly_Dev!S5</f>
+        <v>5.9095327742397785E-8</v>
       </c>
       <c r="T5" s="8">
-        <f>Monthly_Op!T5-Monthly_Op!T5</f>
-        <v>0</v>
+        <f>Monthly_Op!T5-Monthly_Dev!T5</f>
+        <v>1.9299477571621537E-8</v>
       </c>
       <c r="U5" s="8">
-        <f>Monthly_Op!U5-Monthly_Op!U5</f>
-        <v>0</v>
+        <f>Monthly_Op!U5-Monthly_Dev!U5</f>
+        <v>1.1394149623811245E-8</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -6541,80 +6540,80 @@
         <v>44</v>
       </c>
       <c r="C6" s="8">
-        <f>Monthly_Op!C6-Monthly_Op!C6</f>
-        <v>0</v>
+        <f>Monthly_Op!C6-Monthly_Dev!C6</f>
+        <v>6.7984728957526386E-10</v>
       </c>
       <c r="D6" s="8">
-        <f>Monthly_Op!D6-Monthly_Op!D6</f>
-        <v>0</v>
+        <f>Monthly_Op!D6-Monthly_Dev!D6</f>
+        <v>-1.4747477399623676E-4</v>
       </c>
       <c r="E6" s="8">
-        <f>Monthly_Op!E6-Monthly_Op!E6</f>
-        <v>0</v>
+        <f>Monthly_Op!E6-Monthly_Dev!E6</f>
+        <v>-1.6413484047461679E-5</v>
       </c>
       <c r="F6" s="8">
-        <f>Monthly_Op!F6-Monthly_Op!F6</f>
+        <f>Monthly_Op!F6-Monthly_Dev!F6</f>
         <v>0</v>
       </c>
       <c r="G6" s="8">
-        <f>Monthly_Op!G6-Monthly_Op!G6</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="10">
-        <f>Monthly_Op!H6-Monthly_Op!H6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="10">
-        <f>Monthly_Op!I6-Monthly_Op!I6</f>
-        <v>0</v>
+        <f>Monthly_Op!G6-Monthly_Dev!G6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <f>Monthly_Op!H6-Monthly_Dev!H6</f>
+        <v>-4.9137419000544469E-4</v>
+      </c>
+      <c r="I6" s="8">
+        <f>Monthly_Op!I6-Monthly_Dev!I6</f>
+        <v>4.103997956974581E-4</v>
       </c>
       <c r="J6" s="8">
-        <f>Monthly_Op!J6-Monthly_Op!J6</f>
-        <v>0</v>
+        <f>Monthly_Op!J6-Monthly_Dev!J6</f>
+        <v>2.8094859771954361E-11</v>
       </c>
       <c r="K6" s="8">
-        <f>Monthly_Op!K6-Monthly_Op!K6</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="10">
-        <f>Monthly_Op!L6-Monthly_Op!L6</f>
-        <v>0</v>
+        <f>Monthly_Op!K6-Monthly_Dev!K6</f>
+        <v>8.4202156358514912E-10</v>
+      </c>
+      <c r="L6" s="8">
+        <f>Monthly_Op!L6-Monthly_Dev!L6</f>
+        <v>-5.0000157989416039E-3</v>
       </c>
       <c r="M6" s="8">
-        <f>Monthly_Op!M6-Monthly_Op!M6</f>
+        <f>Monthly_Op!M6-Monthly_Dev!M6</f>
         <v>0</v>
       </c>
       <c r="N6" s="8">
-        <f>Monthly_Op!N6-Monthly_Op!N6</f>
-        <v>0</v>
+        <f>Monthly_Op!N6-Monthly_Dev!N6</f>
+        <v>1.0520125215407461E-8</v>
       </c>
       <c r="O6" s="8">
-        <f>Monthly_Op!O6-Monthly_Op!O6</f>
-        <v>0</v>
+        <f>Monthly_Op!O6-Monthly_Dev!O6</f>
+        <v>6.1004357121419162E-10</v>
       </c>
       <c r="P6" s="8">
-        <f>Monthly_Op!P6-Monthly_Op!P6</f>
-        <v>0</v>
+        <f>Monthly_Op!P6-Monthly_Dev!P6</f>
+        <v>-2.8499925974756479E-8</v>
       </c>
       <c r="Q6" s="8">
-        <f>Monthly_Op!Q6-Monthly_Op!Q6</f>
-        <v>0</v>
+        <f>Monthly_Op!Q6-Monthly_Dev!Q6</f>
+        <v>4.400499165058136E-8</v>
       </c>
       <c r="R6" s="8">
-        <f>Monthly_Op!R6-Monthly_Op!R6</f>
-        <v>0</v>
+        <f>Monthly_Op!R6-Monthly_Dev!R6</f>
+        <v>-7.3981937021017075E-8</v>
       </c>
       <c r="S6" s="8">
-        <f>Monthly_Op!S6-Monthly_Op!S6</f>
-        <v>0</v>
+        <f>Monthly_Op!S6-Monthly_Dev!S6</f>
+        <v>-7.2992406785488129E-8</v>
       </c>
       <c r="T6" s="8">
-        <f>Monthly_Op!T6-Monthly_Op!T6</f>
-        <v>0</v>
+        <f>Monthly_Op!T6-Monthly_Dev!T6</f>
+        <v>7.9999153967946768E-9</v>
       </c>
       <c r="U6" s="8">
-        <f>Monthly_Op!U6-Monthly_Op!U6</f>
-        <v>0</v>
+        <f>Monthly_Op!U6-Monthly_Dev!U6</f>
+        <v>3.4997356124222279E-8</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -6625,80 +6624,80 @@
         <v>0</v>
       </c>
       <c r="C7" s="8">
-        <f>Monthly_Op!C7-Monthly_Op!C7</f>
-        <v>0</v>
+        <f>Monthly_Op!C7-Monthly_Dev!C7</f>
+        <v>2.4101609596982598E-9</v>
       </c>
       <c r="D7" s="8">
-        <f>Monthly_Op!D7-Monthly_Op!D7</f>
-        <v>0</v>
+        <f>Monthly_Op!D7-Monthly_Dev!D7</f>
+        <v>2.4852995397850464E-4</v>
       </c>
       <c r="E7" s="8">
-        <f>Monthly_Op!E7-Monthly_Op!E7</f>
-        <v>0</v>
+        <f>Monthly_Op!E7-Monthly_Dev!E7</f>
+        <v>-1.643234099901747E-5</v>
       </c>
       <c r="F7" s="8">
-        <f>Monthly_Op!F7-Monthly_Op!F7</f>
+        <f>Monthly_Op!F7-Monthly_Dev!F7</f>
         <v>0</v>
       </c>
       <c r="G7" s="8">
-        <f>Monthly_Op!G7-Monthly_Op!G7</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="10">
-        <f>Monthly_Op!H7-Monthly_Op!H7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="10">
-        <f>Monthly_Op!I7-Monthly_Op!I7</f>
-        <v>0</v>
+        <f>Monthly_Op!G7-Monthly_Dev!G7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
+        <f>Monthly_Op!H7-Monthly_Dev!H7</f>
+        <v>-4.913249999844993E-4</v>
+      </c>
+      <c r="I7" s="8">
+        <f>Monthly_Op!I7-Monthly_Dev!I7</f>
+        <v>4.1039973960010911E-4</v>
       </c>
       <c r="J7" s="8">
-        <f>Monthly_Op!J7-Monthly_Op!J7</f>
-        <v>0</v>
+        <f>Monthly_Op!J7-Monthly_Dev!J7</f>
+        <v>-2.4698465495021082E-11</v>
       </c>
       <c r="K7" s="8">
-        <f>Monthly_Op!K7-Monthly_Op!K7</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="10">
-        <f>Monthly_Op!L7-Monthly_Op!L7</f>
-        <v>0</v>
+        <f>Monthly_Op!K7-Monthly_Dev!K7</f>
+        <v>-2.1032064978498966E-11</v>
+      </c>
+      <c r="L7" s="8">
+        <f>Monthly_Op!L7-Monthly_Dev!L7</f>
+        <v>-4.9999883995042183E-3</v>
       </c>
       <c r="M7" s="8">
-        <f>Monthly_Op!M7-Monthly_Op!M7</f>
+        <f>Monthly_Op!M7-Monthly_Dev!M7</f>
         <v>0</v>
       </c>
       <c r="N7" s="8">
-        <f>Monthly_Op!N7-Monthly_Op!N7</f>
-        <v>0</v>
+        <f>Monthly_Op!N7-Monthly_Dev!N7</f>
+        <v>1.3870248949388042E-8</v>
       </c>
       <c r="O7" s="8">
-        <f>Monthly_Op!O7-Monthly_Op!O7</f>
-        <v>0</v>
+        <f>Monthly_Op!O7-Monthly_Dev!O7</f>
+        <v>7.3987393989227712E-10</v>
       </c>
       <c r="P7" s="8">
-        <f>Monthly_Op!P7-Monthly_Op!P7</f>
-        <v>0</v>
+        <f>Monthly_Op!P7-Monthly_Dev!P7</f>
+        <v>8.0999598139896989E-9</v>
       </c>
       <c r="Q7" s="8">
-        <f>Monthly_Op!Q7-Monthly_Op!Q7</f>
-        <v>0</v>
+        <f>Monthly_Op!Q7-Monthly_Dev!Q7</f>
+        <v>-6.809714250266552E-7</v>
       </c>
       <c r="R7" s="8">
-        <f>Monthly_Op!R7-Monthly_Op!R7</f>
-        <v>0</v>
+        <f>Monthly_Op!R7-Monthly_Dev!R7</f>
+        <v>-3.2305251806974411E-8</v>
       </c>
       <c r="S7" s="8">
-        <f>Monthly_Op!S7-Monthly_Op!S7</f>
-        <v>0</v>
+        <f>Monthly_Op!S7-Monthly_Dev!S7</f>
+        <v>-8.800998330116272E-8</v>
       </c>
       <c r="T7" s="8">
-        <f>Monthly_Op!T7-Monthly_Op!T7</f>
-        <v>0</v>
+        <f>Monthly_Op!T7-Monthly_Dev!T7</f>
+        <v>-4.0599843487143517E-9</v>
       </c>
       <c r="U7" s="8">
-        <f>Monthly_Op!U7-Monthly_Op!U7</f>
-        <v>0</v>
+        <f>Monthly_Op!U7-Monthly_Dev!U7</f>
+        <v>-1.9994331523776054E-8</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -6709,80 +6708,80 @@
         <v>46</v>
       </c>
       <c r="C8" s="8">
-        <f>Monthly_Op!C8-Monthly_Op!C8</f>
-        <v>0</v>
+        <f>Monthly_Op!C8-Monthly_Dev!C8</f>
+        <v>3.4997356124222279E-9</v>
       </c>
       <c r="D8" s="8">
-        <f>Monthly_Op!D8-Monthly_Op!D8</f>
-        <v>0</v>
+        <f>Monthly_Op!D8-Monthly_Dev!D8</f>
+        <v>4.8128359500765328E-4</v>
       </c>
       <c r="E8" s="8">
-        <f>Monthly_Op!E8-Monthly_Op!E8</f>
-        <v>0</v>
+        <f>Monthly_Op!E8-Monthly_Dev!E8</f>
+        <v>-1.6447062023416947E-5</v>
       </c>
       <c r="F8" s="8">
-        <f>Monthly_Op!F8-Monthly_Op!F8</f>
+        <f>Monthly_Op!F8-Monthly_Dev!F8</f>
         <v>0</v>
       </c>
       <c r="G8" s="8">
-        <f>Monthly_Op!G8-Monthly_Op!G8</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="10">
-        <f>Monthly_Op!H8-Monthly_Op!H8</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="10">
-        <f>Monthly_Op!I8-Monthly_Op!I8</f>
-        <v>0</v>
+        <f>Monthly_Op!G8-Monthly_Dev!G8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
+        <f>Monthly_Op!H8-Monthly_Dev!H8</f>
+        <v>-4.9117487014882499E-4</v>
+      </c>
+      <c r="I8" s="8">
+        <f>Monthly_Op!I8-Monthly_Dev!I8</f>
+        <v>4.1039976449752658E-4</v>
       </c>
       <c r="J8" s="8">
-        <f>Monthly_Op!J8-Monthly_Op!J8</f>
-        <v>0</v>
+        <f>Monthly_Op!J8-Monthly_Dev!J8</f>
+        <v>-5.6985527407960035E-12</v>
       </c>
       <c r="K8" s="8">
-        <f>Monthly_Op!K8-Monthly_Op!K8</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="10">
-        <f>Monthly_Op!L8-Monthly_Op!L8</f>
-        <v>0</v>
+        <f>Monthly_Op!K8-Monthly_Dev!K8</f>
+        <v>-1.6103740563266911E-10</v>
+      </c>
+      <c r="L8" s="8">
+        <f>Monthly_Op!L8-Monthly_Dev!L8</f>
+        <v>-4.9999836992355995E-3</v>
       </c>
       <c r="M8" s="8">
-        <f>Monthly_Op!M8-Monthly_Op!M8</f>
+        <f>Monthly_Op!M8-Monthly_Dev!M8</f>
         <v>0</v>
       </c>
       <c r="N8" s="8">
-        <f>Monthly_Op!N8-Monthly_Op!N8</f>
-        <v>0</v>
+        <f>Monthly_Op!N8-Monthly_Dev!N8</f>
+        <v>-2.8599060897249728E-9</v>
       </c>
       <c r="O8" s="8">
-        <f>Monthly_Op!O8-Monthly_Op!O8</f>
-        <v>0</v>
+        <f>Monthly_Op!O8-Monthly_Dev!O8</f>
+        <v>-5.0999915401916951E-10</v>
       </c>
       <c r="P8" s="8">
-        <f>Monthly_Op!P8-Monthly_Op!P8</f>
-        <v>0</v>
+        <f>Monthly_Op!P8-Monthly_Dev!P8</f>
+        <v>9.4005372375249863E-9</v>
       </c>
       <c r="Q8" s="8">
-        <f>Monthly_Op!Q8-Monthly_Op!Q8</f>
-        <v>0</v>
+        <f>Monthly_Op!Q8-Monthly_Dev!Q8</f>
+        <v>-4.7030043788254261E-6</v>
       </c>
       <c r="R8" s="8">
-        <f>Monthly_Op!R8-Monthly_Op!R8</f>
-        <v>0</v>
+        <f>Monthly_Op!R8-Monthly_Dev!R8</f>
+        <v>-7.8100129030644894E-8</v>
       </c>
       <c r="S8" s="8">
-        <f>Monthly_Op!S8-Monthly_Op!S8</f>
-        <v>0</v>
+        <f>Monthly_Op!S8-Monthly_Dev!S8</f>
+        <v>-1.2907548807561398E-8</v>
       </c>
       <c r="T8" s="8">
-        <f>Monthly_Op!T8-Monthly_Op!T8</f>
-        <v>0</v>
+        <f>Monthly_Op!T8-Monthly_Dev!T8</f>
+        <v>-3.9999576983973384E-9</v>
       </c>
       <c r="U8" s="8">
-        <f>Monthly_Op!U8-Monthly_Op!U8</f>
-        <v>0</v>
+        <f>Monthly_Op!U8-Monthly_Dev!U8</f>
+        <v>-4.560992238111794E-6</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -6793,80 +6792,80 @@
         <v>46</v>
       </c>
       <c r="C9" s="8">
-        <f>Monthly_Op!C9-Monthly_Op!C9</f>
-        <v>0</v>
+        <f>Monthly_Op!C9-Monthly_Dev!C9</f>
+        <v>-7.6988726505078375E-10</v>
       </c>
       <c r="D9" s="8">
-        <f>Monthly_Op!D9-Monthly_Op!D9</f>
-        <v>0</v>
+        <f>Monthly_Op!D9-Monthly_Dev!D9</f>
+        <v>3.1283310801200059E-4</v>
       </c>
       <c r="E9" s="8">
-        <f>Monthly_Op!E9-Monthly_Op!E9</f>
-        <v>0</v>
+        <f>Monthly_Op!E9-Monthly_Dev!E9</f>
+        <v>-1.6487058019265532E-5</v>
       </c>
       <c r="F9" s="8">
-        <f>Monthly_Op!F9-Monthly_Op!F9</f>
+        <f>Monthly_Op!F9-Monthly_Dev!F9</f>
         <v>0</v>
       </c>
       <c r="G9" s="8">
-        <f>Monthly_Op!G9-Monthly_Op!G9</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="10">
-        <f>Monthly_Op!H9-Monthly_Op!H9</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="10">
-        <f>Monthly_Op!I9-Monthly_Op!I9</f>
-        <v>0</v>
+        <f>Monthly_Op!G9-Monthly_Dev!G9</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
+        <f>Monthly_Op!H9-Monthly_Dev!H9</f>
+        <v>-4.909334102194407E-4</v>
+      </c>
+      <c r="I9" s="8">
+        <f>Monthly_Op!I9-Monthly_Dev!I9</f>
+        <v>4.1039978950152545E-4</v>
       </c>
       <c r="J9" s="8">
-        <f>Monthly_Op!J9-Monthly_Op!J9</f>
-        <v>0</v>
+        <f>Monthly_Op!J9-Monthly_Dev!J9</f>
+        <v>-2.4698465495021082E-11</v>
       </c>
       <c r="K9" s="8">
-        <f>Monthly_Op!K9-Monthly_Op!K9</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="10">
-        <f>Monthly_Op!L9-Monthly_Op!L9</f>
-        <v>0</v>
+        <f>Monthly_Op!K9-Monthly_Dev!K9</f>
+        <v>1.8502532839193009E-10</v>
+      </c>
+      <c r="L9" s="8">
+        <f>Monthly_Op!L9-Monthly_Dev!L9</f>
+        <v>-5.0000240007648245E-3</v>
       </c>
       <c r="M9" s="8">
-        <f>Monthly_Op!M9-Monthly_Op!M9</f>
+        <f>Monthly_Op!M9-Monthly_Dev!M9</f>
         <v>0</v>
       </c>
       <c r="N9" s="8">
-        <f>Monthly_Op!N9-Monthly_Op!N9</f>
-        <v>0</v>
+        <f>Monthly_Op!N9-Monthly_Dev!N9</f>
+        <v>2.7002897695638239E-9</v>
       </c>
       <c r="O9" s="8">
-        <f>Monthly_Op!O9-Monthly_Op!O9</f>
-        <v>0</v>
+        <f>Monthly_Op!O9-Monthly_Dev!O9</f>
+        <v>1.0400071914773434E-9</v>
       </c>
       <c r="P9" s="8">
-        <f>Monthly_Op!P9-Monthly_Op!P9</f>
-        <v>0</v>
+        <f>Monthly_Op!P9-Monthly_Dev!P9</f>
+        <v>-1.3098542694933712E-8</v>
       </c>
       <c r="Q9" s="8">
-        <f>Monthly_Op!Q9-Monthly_Op!Q9</f>
-        <v>0</v>
+        <f>Monthly_Op!Q9-Monthly_Dev!Q9</f>
+        <v>1.1239899322390556E-6</v>
       </c>
       <c r="R9" s="8">
-        <f>Monthly_Op!R9-Monthly_Op!R9</f>
-        <v>0</v>
+        <f>Monthly_Op!R9-Monthly_Dev!R9</f>
+        <v>6.7404471337795258E-8</v>
       </c>
       <c r="S9" s="8">
-        <f>Monthly_Op!S9-Monthly_Op!S9</f>
-        <v>0</v>
+        <f>Monthly_Op!S9-Monthly_Dev!S9</f>
+        <v>-4.0399754652753472E-8</v>
       </c>
       <c r="T9" s="8">
-        <f>Monthly_Op!T9-Monthly_Op!T9</f>
-        <v>0</v>
+        <f>Monthly_Op!T9-Monthly_Dev!T9</f>
+        <v>-5.398760549724102E-9</v>
       </c>
       <c r="U9" s="8">
-        <f>Monthly_Op!U9-Monthly_Op!U9</f>
-        <v>0</v>
+        <f>Monthly_Op!U9-Monthly_Dev!U9</f>
+        <v>3.3702235668897629E-7</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -6877,80 +6876,80 @@
         <v>45</v>
       </c>
       <c r="C10" s="8">
-        <f>Monthly_Op!C10-Monthly_Op!C10</f>
-        <v>0</v>
+        <f>Monthly_Op!C10-Monthly_Dev!C10</f>
+        <v>-1.3601493265014142E-9</v>
       </c>
       <c r="D10" s="8">
-        <f>Monthly_Op!D10-Monthly_Op!D10</f>
-        <v>0</v>
+        <f>Monthly_Op!D10-Monthly_Dev!D10</f>
+        <v>3.0668854999760242E-4</v>
       </c>
       <c r="E10" s="8">
-        <f>Monthly_Op!E10-Monthly_Op!E10</f>
-        <v>0</v>
+        <f>Monthly_Op!E10-Monthly_Dev!E10</f>
+        <v>-1.6572170977724454E-5</v>
       </c>
       <c r="F10" s="8">
-        <f>Monthly_Op!F10-Monthly_Op!F10</f>
+        <f>Monthly_Op!F10-Monthly_Dev!F10</f>
         <v>0</v>
       </c>
       <c r="G10" s="8">
-        <f>Monthly_Op!G10-Monthly_Op!G10</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="10">
-        <f>Monthly_Op!H10-Monthly_Op!H10</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="10">
-        <f>Monthly_Op!I10-Monthly_Op!I10</f>
-        <v>0</v>
+        <f>Monthly_Op!G10-Monthly_Dev!G10</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
+        <f>Monthly_Op!H10-Monthly_Dev!H10</f>
+        <v>-4.9046318008549861E-4</v>
+      </c>
+      <c r="I10" s="8">
+        <f>Monthly_Op!I10-Monthly_Dev!I10</f>
+        <v>4.103997932034531E-4</v>
       </c>
       <c r="J10" s="8">
-        <f>Monthly_Op!J10-Monthly_Op!J10</f>
-        <v>0</v>
+        <f>Monthly_Op!J10-Monthly_Dev!J10</f>
+        <v>-3.9399594697897555E-11</v>
       </c>
       <c r="K10" s="8">
-        <f>Monthly_Op!K10-Monthly_Op!K10</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="10">
-        <f>Monthly_Op!L10-Monthly_Op!L10</f>
-        <v>0</v>
+        <f>Monthly_Op!K10-Monthly_Dev!K10</f>
+        <v>4.0097347664413974E-10</v>
+      </c>
+      <c r="L10" s="8">
+        <f>Monthly_Op!L10-Monthly_Dev!L10</f>
+        <v>-4.9999667589872843E-3</v>
       </c>
       <c r="M10" s="8">
-        <f>Monthly_Op!M10-Monthly_Op!M10</f>
+        <f>Monthly_Op!M10-Monthly_Dev!M10</f>
         <v>0</v>
       </c>
       <c r="N10" s="8">
-        <f>Monthly_Op!N10-Monthly_Op!N10</f>
-        <v>0</v>
+        <f>Monthly_Op!N10-Monthly_Dev!N10</f>
+        <v>1.448006514692679E-8</v>
       </c>
       <c r="O10" s="8">
-        <f>Monthly_Op!O10-Monthly_Op!O10</f>
-        <v>0</v>
+        <f>Monthly_Op!O10-Monthly_Dev!O10</f>
+        <v>2.4988366931211203E-10</v>
       </c>
       <c r="P10" s="8">
-        <f>Monthly_Op!P10-Monthly_Op!P10</f>
-        <v>0</v>
+        <f>Monthly_Op!P10-Monthly_Dev!P10</f>
+        <v>1.7700585885904729E-8</v>
       </c>
       <c r="Q10" s="8">
-        <f>Monthly_Op!Q10-Monthly_Op!Q10</f>
-        <v>0</v>
+        <f>Monthly_Op!Q10-Monthly_Dev!Q10</f>
+        <v>2.4309847503900528E-6</v>
       </c>
       <c r="R10" s="8">
-        <f>Monthly_Op!R10-Monthly_Op!R10</f>
-        <v>0</v>
+        <f>Monthly_Op!R10-Monthly_Dev!R10</f>
+        <v>4.5984052121639252E-8</v>
       </c>
       <c r="S10" s="8">
-        <f>Monthly_Op!S10-Monthly_Op!S10</f>
-        <v>0</v>
+        <f>Monthly_Op!S10-Monthly_Dev!S10</f>
+        <v>5.1193637773394585E-8</v>
       </c>
       <c r="T10" s="8">
-        <f>Monthly_Op!T10-Monthly_Op!T10</f>
-        <v>0</v>
+        <f>Monthly_Op!T10-Monthly_Dev!T10</f>
+        <v>5.2987161325290799E-9</v>
       </c>
       <c r="U10" s="8">
-        <f>Monthly_Op!U10-Monthly_Op!U10</f>
-        <v>0</v>
+        <f>Monthly_Op!U10-Monthly_Dev!U10</f>
+        <v>5.4002157412469387E-7</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -6961,80 +6960,80 @@
         <v>1</v>
       </c>
       <c r="C11" s="8">
-        <f>Monthly_Op!C11-Monthly_Op!C11</f>
-        <v>0</v>
+        <f>Monthly_Op!C11-Monthly_Dev!C11</f>
+        <v>-2.8999238566029817E-9</v>
       </c>
       <c r="D11" s="8">
-        <f>Monthly_Op!D11-Monthly_Op!D11</f>
-        <v>0</v>
+        <f>Monthly_Op!D11-Monthly_Dev!D11</f>
+        <v>3.0600195800900565E-4</v>
       </c>
       <c r="E11" s="8">
-        <f>Monthly_Op!E11-Monthly_Op!E11</f>
-        <v>0</v>
+        <f>Monthly_Op!E11-Monthly_Dev!E11</f>
+        <v>-1.6638217005038314E-5</v>
       </c>
       <c r="F11" s="8">
-        <f>Monthly_Op!F11-Monthly_Op!F11</f>
+        <f>Monthly_Op!F11-Monthly_Dev!F11</f>
         <v>0</v>
       </c>
       <c r="G11" s="8">
-        <f>Monthly_Op!G11-Monthly_Op!G11</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="10">
-        <f>Monthly_Op!H11-Monthly_Op!H11</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="10">
-        <f>Monthly_Op!I11-Monthly_Op!I11</f>
-        <v>0</v>
+        <f>Monthly_Op!G11-Monthly_Dev!G11</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="8">
+        <f>Monthly_Op!H11-Monthly_Dev!H11</f>
+        <v>-4.8975137997331331E-4</v>
+      </c>
+      <c r="I11" s="8">
+        <f>Monthly_Op!I11-Monthly_Dev!I11</f>
+        <v>4.1039978519563647E-4</v>
       </c>
       <c r="J11" s="8">
-        <f>Monthly_Op!J11-Monthly_Op!J11</f>
-        <v>0</v>
+        <f>Monthly_Op!J11-Monthly_Dev!J11</f>
+        <v>-2.3803181647963356E-11</v>
       </c>
       <c r="K11" s="8">
-        <f>Monthly_Op!K11-Monthly_Op!K11</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="10">
-        <f>Monthly_Op!L11-Monthly_Op!L11</f>
-        <v>0</v>
+        <f>Monthly_Op!K11-Monthly_Dev!K11</f>
+        <v>-7.9796791396802291E-10</v>
+      </c>
+      <c r="L11" s="8">
+        <f>Monthly_Op!L11-Monthly_Dev!L11</f>
+        <v>-5.0000212704617297E-3</v>
       </c>
       <c r="M11" s="8">
-        <f>Monthly_Op!M11-Monthly_Op!M11</f>
+        <f>Monthly_Op!M11-Monthly_Dev!M11</f>
         <v>0</v>
       </c>
       <c r="N11" s="8">
-        <f>Monthly_Op!N11-Monthly_Op!N11</f>
-        <v>0</v>
+        <f>Monthly_Op!N11-Monthly_Dev!N11</f>
+        <v>7.8798620961606503E-9</v>
       </c>
       <c r="O11" s="8">
-        <f>Monthly_Op!O11-Monthly_Op!O11</f>
-        <v>0</v>
+        <f>Monthly_Op!O11-Monthly_Dev!O11</f>
+        <v>-4.2996362026315182E-10</v>
       </c>
       <c r="P11" s="8">
-        <f>Monthly_Op!P11-Monthly_Op!P11</f>
-        <v>0</v>
+        <f>Monthly_Op!P11-Monthly_Dev!P11</f>
+        <v>-1.2930104276165366E-7</v>
       </c>
       <c r="Q11" s="8">
-        <f>Monthly_Op!Q11-Monthly_Op!Q11</f>
-        <v>0</v>
+        <f>Monthly_Op!Q11-Monthly_Dev!Q11</f>
+        <v>9.2269969172775745E-5</v>
       </c>
       <c r="R11" s="8">
-        <f>Monthly_Op!R11-Monthly_Op!R11</f>
-        <v>0</v>
+        <f>Monthly_Op!R11-Monthly_Dev!R11</f>
+        <v>-6.3009792938828468E-8</v>
       </c>
       <c r="S11" s="8">
-        <f>Monthly_Op!S11-Monthly_Op!S11</f>
-        <v>0</v>
+        <f>Monthly_Op!S11-Monthly_Dev!S11</f>
+        <v>6.3009792938828468E-9</v>
       </c>
       <c r="T11" s="8">
-        <f>Monthly_Op!T11-Monthly_Op!T11</f>
-        <v>0</v>
+        <f>Monthly_Op!T11-Monthly_Dev!T11</f>
+        <v>1.1968950275331736E-9</v>
       </c>
       <c r="U11" s="8">
-        <f>Monthly_Op!U11-Monthly_Op!U11</f>
-        <v>0</v>
+        <f>Monthly_Op!U11-Monthly_Dev!U11</f>
+        <v>4.900200292468071E-5</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -7045,80 +7044,80 @@
         <v>44</v>
       </c>
       <c r="C12" s="8">
-        <f>Monthly_Op!C12-Monthly_Op!C12</f>
-        <v>0</v>
+        <f>Monthly_Op!C12-Monthly_Dev!C12</f>
+        <v>1.9299477571621537E-9</v>
       </c>
       <c r="D12" s="8">
-        <f>Monthly_Op!D12-Monthly_Op!D12</f>
-        <v>0</v>
+        <f>Monthly_Op!D12-Monthly_Dev!D12</f>
+        <v>-1.5725839000424457E-4</v>
       </c>
       <c r="E12" s="8">
-        <f>Monthly_Op!E12-Monthly_Op!E12</f>
-        <v>0</v>
+        <f>Monthly_Op!E12-Monthly_Dev!E12</f>
+        <v>-1.6776697975728894E-5</v>
       </c>
       <c r="F12" s="8">
-        <f>Monthly_Op!F12-Monthly_Op!F12</f>
+        <f>Monthly_Op!F12-Monthly_Dev!F12</f>
         <v>0</v>
       </c>
       <c r="G12" s="8">
-        <f>Monthly_Op!G12-Monthly_Op!G12</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="10">
-        <f>Monthly_Op!H12-Monthly_Op!H12</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="10">
-        <f>Monthly_Op!I12-Monthly_Op!I12</f>
-        <v>0</v>
+        <f>Monthly_Op!G12-Monthly_Dev!G12</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
+        <f>Monthly_Op!H12-Monthly_Dev!H12</f>
+        <v>-4.8842666001291946E-4</v>
+      </c>
+      <c r="I12" s="8">
+        <f>Monthly_Op!I12-Monthly_Dev!I12</f>
+        <v>4.1039976679968504E-4</v>
       </c>
       <c r="J12" s="8">
-        <f>Monthly_Op!J12-Monthly_Op!J12</f>
-        <v>0</v>
+        <f>Monthly_Op!J12-Monthly_Dev!J12</f>
+        <v>1.1340262062731199E-10</v>
       </c>
       <c r="K12" s="8">
-        <f>Monthly_Op!K12-Monthly_Op!K12</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="10">
-        <f>Monthly_Op!L12-Monthly_Op!L12</f>
-        <v>0</v>
+        <f>Monthly_Op!K12-Monthly_Dev!K12</f>
+        <v>9.4996721600182354E-10</v>
+      </c>
+      <c r="L12" s="8">
+        <f>Monthly_Op!L12-Monthly_Dev!L12</f>
+        <v>-4.9999916991509963E-3</v>
       </c>
       <c r="M12" s="8">
-        <f>Monthly_Op!M12-Monthly_Op!M12</f>
+        <f>Monthly_Op!M12-Monthly_Dev!M12</f>
         <v>0</v>
       </c>
       <c r="N12" s="8">
-        <f>Monthly_Op!N12-Monthly_Op!N12</f>
-        <v>0</v>
+        <f>Monthly_Op!N12-Monthly_Dev!N12</f>
+        <v>9.0499270299915224E-9</v>
       </c>
       <c r="O12" s="8">
-        <f>Monthly_Op!O12-Monthly_Op!O12</f>
-        <v>0</v>
+        <f>Monthly_Op!O12-Monthly_Dev!O12</f>
+        <v>-1.4401848602574319E-9</v>
       </c>
       <c r="P12" s="8">
-        <f>Monthly_Op!P12-Monthly_Op!P12</f>
-        <v>0</v>
+        <f>Monthly_Op!P12-Monthly_Dev!P12</f>
+        <v>-1.0780058801174164E-7</v>
       </c>
       <c r="Q12" s="8">
-        <f>Monthly_Op!Q12-Monthly_Op!Q12</f>
-        <v>0</v>
+        <f>Monthly_Op!Q12-Monthly_Dev!Q12</f>
+        <v>9.6770236268639565E-6</v>
       </c>
       <c r="R12" s="8">
-        <f>Monthly_Op!R12-Monthly_Op!R12</f>
-        <v>0</v>
+        <f>Monthly_Op!R12-Monthly_Dev!R12</f>
+        <v>1.2980308383703232E-8</v>
       </c>
       <c r="S12" s="8">
-        <f>Monthly_Op!S12-Monthly_Op!S12</f>
-        <v>0</v>
+        <f>Monthly_Op!S12-Monthly_Dev!S12</f>
+        <v>5.0393282435834408E-8</v>
       </c>
       <c r="T12" s="8">
-        <f>Monthly_Op!T12-Monthly_Op!T12</f>
-        <v>0</v>
+        <f>Monthly_Op!T12-Monthly_Dev!T12</f>
+        <v>8.1599864643067122E-8</v>
       </c>
       <c r="U12" s="8">
-        <f>Monthly_Op!U12-Monthly_Op!U12</f>
-        <v>0</v>
+        <f>Monthly_Op!U12-Monthly_Dev!U12</f>
+        <v>3.8699363358318806E-7</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -7129,80 +7128,80 @@
         <v>45</v>
       </c>
       <c r="C13" s="8">
-        <f>Monthly_Op!C13-Monthly_Op!C13</f>
-        <v>0</v>
+        <f>Monthly_Op!C13-Monthly_Dev!C13</f>
+        <v>-1.9099388737231493E-9</v>
       </c>
       <c r="D13" s="8">
-        <f>Monthly_Op!D13-Monthly_Op!D13</f>
-        <v>0</v>
+        <f>Monthly_Op!D13-Monthly_Dev!D13</f>
+        <v>-8.8503665904227091E-4</v>
       </c>
       <c r="E13" s="8">
-        <f>Monthly_Op!E13-Monthly_Op!E13</f>
-        <v>0</v>
+        <f>Monthly_Op!E13-Monthly_Dev!E13</f>
+        <v>-1.7006556049636856E-5</v>
       </c>
       <c r="F13" s="8">
-        <f>Monthly_Op!F13-Monthly_Op!F13</f>
+        <f>Monthly_Op!F13-Monthly_Dev!F13</f>
         <v>0</v>
       </c>
       <c r="G13" s="8">
-        <f>Monthly_Op!G13-Monthly_Op!G13</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="10">
-        <f>Monthly_Op!H13-Monthly_Op!H13</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="10">
-        <f>Monthly_Op!I13-Monthly_Op!I13</f>
-        <v>0</v>
+        <f>Monthly_Op!G13-Monthly_Dev!G13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
+        <f>Monthly_Op!H13-Monthly_Dev!H13</f>
+        <v>-4.8680432018954889E-4</v>
+      </c>
+      <c r="I13" s="8">
+        <f>Monthly_Op!I13-Monthly_Dev!I13</f>
+        <v>4.1039980290236144E-4</v>
       </c>
       <c r="J13" s="8">
-        <f>Monthly_Op!J13-Monthly_Op!J13</f>
-        <v>0</v>
+        <f>Monthly_Op!J13-Monthly_Dev!J13</f>
+        <v>3.5900882267014822E-10</v>
       </c>
       <c r="K13" s="8">
-        <f>Monthly_Op!K13-Monthly_Op!K13</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="10">
-        <f>Monthly_Op!L13-Monthly_Op!L13</f>
-        <v>0</v>
+        <f>Monthly_Op!K13-Monthly_Dev!K13</f>
+        <v>-8.4037310443818569E-10</v>
+      </c>
+      <c r="L13" s="8">
+        <f>Monthly_Op!L13-Monthly_Dev!L13</f>
+        <v>-4.999997900085873E-3</v>
       </c>
       <c r="M13" s="8">
-        <f>Monthly_Op!M13-Monthly_Op!M13</f>
+        <f>Monthly_Op!M13-Monthly_Dev!M13</f>
         <v>0</v>
       </c>
       <c r="N13" s="8">
-        <f>Monthly_Op!N13-Monthly_Op!N13</f>
-        <v>0</v>
+        <f>Monthly_Op!N13-Monthly_Dev!N13</f>
+        <v>-1.6410012904088944E-8</v>
       </c>
       <c r="O13" s="8">
-        <f>Monthly_Op!O13-Monthly_Op!O13</f>
-        <v>0</v>
+        <f>Monthly_Op!O13-Monthly_Dev!O13</f>
+        <v>-1.210082700708881E-9</v>
       </c>
       <c r="P13" s="8">
-        <f>Monthly_Op!P13-Monthly_Op!P13</f>
-        <v>0</v>
+        <f>Monthly_Op!P13-Monthly_Dev!P13</f>
+        <v>-7.2299371822737157E-8</v>
       </c>
       <c r="Q13" s="8">
-        <f>Monthly_Op!Q13-Monthly_Op!Q13</f>
-        <v>0</v>
+        <f>Monthly_Op!Q13-Monthly_Dev!Q13</f>
+        <v>-5.7107070460915565E-5</v>
       </c>
       <c r="R13" s="8">
-        <f>Monthly_Op!R13-Monthly_Op!R13</f>
-        <v>0</v>
+        <f>Monthly_Op!R13-Monthly_Dev!R13</f>
+        <v>-1.8801074475049973E-8</v>
       </c>
       <c r="S13" s="8">
-        <f>Monthly_Op!S13-Monthly_Op!S13</f>
-        <v>0</v>
+        <f>Monthly_Op!S13-Monthly_Dev!S13</f>
+        <v>-2.5596818886697292E-8</v>
       </c>
       <c r="T13" s="8">
-        <f>Monthly_Op!T13-Monthly_Op!T13</f>
-        <v>0</v>
+        <f>Monthly_Op!T13-Monthly_Dev!T13</f>
+        <v>-2.7899659471586347E-8</v>
       </c>
       <c r="U13" s="8">
-        <f>Monthly_Op!U13-Monthly_Op!U13</f>
-        <v>0</v>
+        <f>Monthly_Op!U13-Monthly_Dev!U13</f>
+        <v>-4.4910120777785778E-6</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -7213,80 +7212,80 @@
         <v>2</v>
       </c>
       <c r="C14" s="8">
-        <f>Monthly_Op!C14-Monthly_Op!C14</f>
-        <v>0</v>
+        <f>Monthly_Op!C14-Monthly_Dev!C14</f>
+        <v>3.0299815989565104E-9</v>
       </c>
       <c r="D14" s="8">
-        <f>Monthly_Op!D14-Monthly_Op!D14</f>
-        <v>0</v>
+        <f>Monthly_Op!D14-Monthly_Dev!D14</f>
+        <v>-9.8500173402271685E-4</v>
       </c>
       <c r="E14" s="8">
-        <f>Monthly_Op!E14-Monthly_Op!E14</f>
-        <v>0</v>
+        <f>Monthly_Op!E14-Monthly_Dev!E14</f>
+        <v>-1.7148686083601206E-5</v>
       </c>
       <c r="F14" s="8">
-        <f>Monthly_Op!F14-Monthly_Op!F14</f>
+        <f>Monthly_Op!F14-Monthly_Dev!F14</f>
         <v>0</v>
       </c>
       <c r="G14" s="8">
-        <f>Monthly_Op!G14-Monthly_Op!G14</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="10">
-        <f>Monthly_Op!H14-Monthly_Op!H14</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="10">
-        <f>Monthly_Op!I14-Monthly_Op!I14</f>
-        <v>0</v>
+        <f>Monthly_Op!G14-Monthly_Dev!G14</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
+        <f>Monthly_Op!H14-Monthly_Dev!H14</f>
+        <v>-4.8584887008473743E-4</v>
+      </c>
+      <c r="I14" s="8">
+        <f>Monthly_Op!I14-Monthly_Dev!I14</f>
+        <v>4.1039976550649726E-4</v>
       </c>
       <c r="J14" s="8">
-        <f>Monthly_Op!J14-Monthly_Op!J14</f>
-        <v>0</v>
+        <f>Monthly_Op!J14-Monthly_Dev!J14</f>
+        <v>7.8998141361807939E-11</v>
       </c>
       <c r="K14" s="8">
-        <f>Monthly_Op!K14-Monthly_Op!K14</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="10">
-        <f>Monthly_Op!L14-Monthly_Op!L14</f>
-        <v>0</v>
+        <f>Monthly_Op!K14-Monthly_Dev!K14</f>
+        <v>-5.4603788157692179E-10</v>
+      </c>
+      <c r="L14" s="8">
+        <f>Monthly_Op!L14-Monthly_Dev!L14</f>
+        <v>-5.0000110004475573E-3</v>
       </c>
       <c r="M14" s="8">
-        <f>Monthly_Op!M14-Monthly_Op!M14</f>
+        <f>Monthly_Op!M14-Monthly_Dev!M14</f>
         <v>0</v>
       </c>
       <c r="N14" s="8">
-        <f>Monthly_Op!N14-Monthly_Op!N14</f>
-        <v>0</v>
+        <f>Monthly_Op!N14-Monthly_Dev!N14</f>
+        <v>-4.0599843487143517E-9</v>
       </c>
       <c r="O14" s="8">
-        <f>Monthly_Op!O14-Monthly_Op!O14</f>
-        <v>0</v>
+        <f>Monthly_Op!O14-Monthly_Dev!O14</f>
+        <v>-4.8999027058016509E-10</v>
       </c>
       <c r="P14" s="8">
-        <f>Monthly_Op!P14-Monthly_Op!P14</f>
-        <v>0</v>
+        <f>Monthly_Op!P14-Monthly_Dev!P14</f>
+        <v>-1.1890006135217845E-7</v>
       </c>
       <c r="Q14" s="8">
-        <f>Monthly_Op!Q14-Monthly_Op!Q14</f>
-        <v>0</v>
+        <f>Monthly_Op!Q14-Monthly_Dev!Q14</f>
+        <v>4.8757996410131454E-5</v>
       </c>
       <c r="R14" s="8">
-        <f>Monthly_Op!R14-Monthly_Op!R14</f>
-        <v>0</v>
+        <f>Monthly_Op!R14-Monthly_Dev!R14</f>
+        <v>8.1505277194082737E-8</v>
       </c>
       <c r="S14" s="8">
-        <f>Monthly_Op!S14-Monthly_Op!S14</f>
-        <v>0</v>
+        <f>Monthly_Op!S14-Monthly_Dev!S14</f>
+        <v>-7.2206603363156319E-8</v>
       </c>
       <c r="T14" s="8">
-        <f>Monthly_Op!T14-Monthly_Op!T14</f>
-        <v>0</v>
+        <f>Monthly_Op!T14-Monthly_Dev!T14</f>
+        <v>-4.0599843487143517E-8</v>
       </c>
       <c r="U14" s="8">
-        <f>Monthly_Op!U14-Monthly_Op!U14</f>
-        <v>0</v>
+        <f>Monthly_Op!U14-Monthly_Dev!U14</f>
+        <v>4.8996997065842152E-5</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -7297,80 +7296,80 @@
         <v>47</v>
       </c>
       <c r="C15" s="8">
-        <f>Monthly_Op!C15-Monthly_Op!C15</f>
-        <v>0</v>
+        <f>Monthly_Op!C15-Monthly_Dev!C15</f>
+        <v>-2.1200321498326957E-9</v>
       </c>
       <c r="D15" s="8">
-        <f>Monthly_Op!D15-Monthly_Op!D15</f>
-        <v>0</v>
+        <f>Monthly_Op!D15-Monthly_Dev!D15</f>
+        <v>-9.8263929396580352E-4</v>
       </c>
       <c r="E15" s="8">
-        <f>Monthly_Op!E15-Monthly_Op!E15</f>
-        <v>0</v>
+        <f>Monthly_Op!E15-Monthly_Dev!E15</f>
+        <v>-1.7212119018950034E-5</v>
       </c>
       <c r="F15" s="8">
-        <f>Monthly_Op!F15-Monthly_Op!F15</f>
+        <f>Monthly_Op!F15-Monthly_Dev!F15</f>
         <v>0</v>
       </c>
       <c r="G15" s="8">
-        <f>Monthly_Op!G15-Monthly_Op!G15</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="10">
-        <f>Monthly_Op!H15-Monthly_Op!H15</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="10">
-        <f>Monthly_Op!I15-Monthly_Op!I15</f>
-        <v>0</v>
+        <f>Monthly_Op!G15-Monthly_Dev!G15</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
+        <f>Monthly_Op!H15-Monthly_Dev!H15</f>
+        <v>-4.8531676020502346E-4</v>
+      </c>
+      <c r="I15" s="8">
+        <f>Monthly_Op!I15-Monthly_Dev!I15</f>
+        <v>4.1039978400192467E-4</v>
       </c>
       <c r="J15" s="8">
-        <f>Monthly_Op!J15-Monthly_Op!J15</f>
-        <v>0</v>
+        <f>Monthly_Op!J15-Monthly_Dev!J15</f>
+        <v>1.6079582110251067E-10</v>
       </c>
       <c r="K15" s="8">
-        <f>Monthly_Op!K15-Monthly_Op!K15</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="10">
-        <f>Monthly_Op!L15-Monthly_Op!L15</f>
-        <v>0</v>
+        <f>Monthly_Op!K15-Monthly_Dev!K15</f>
+        <v>9.6702024166006595E-10</v>
+      </c>
+      <c r="L15" s="8">
+        <f>Monthly_Op!L15-Monthly_Dev!L15</f>
+        <v>-4.9999709990515839E-3</v>
       </c>
       <c r="M15" s="8">
-        <f>Monthly_Op!M15-Monthly_Op!M15</f>
+        <f>Monthly_Op!M15-Monthly_Dev!M15</f>
         <v>0</v>
       </c>
       <c r="N15" s="8">
-        <f>Monthly_Op!N15-Monthly_Op!N15</f>
-        <v>0</v>
+        <f>Monthly_Op!N15-Monthly_Dev!N15</f>
+        <v>-5.7898432714864612E-9</v>
       </c>
       <c r="O15" s="8">
-        <f>Monthly_Op!O15-Monthly_Op!O15</f>
-        <v>0</v>
+        <f>Monthly_Op!O15-Monthly_Dev!O15</f>
+        <v>-2.2598669602302834E-9</v>
       </c>
       <c r="P15" s="8">
-        <f>Monthly_Op!P15-Monthly_Op!P15</f>
-        <v>0</v>
+        <f>Monthly_Op!P15-Monthly_Dev!P15</f>
+        <v>-1.4180113794282079E-7</v>
       </c>
       <c r="Q15" s="8">
-        <f>Monthly_Op!Q15-Monthly_Op!Q15</f>
-        <v>0</v>
+        <f>Monthly_Op!Q15-Monthly_Dev!Q15</f>
+        <v>6.1100581660866737E-6</v>
       </c>
       <c r="R15" s="8">
-        <f>Monthly_Op!R15-Monthly_Op!R15</f>
-        <v>0</v>
+        <f>Monthly_Op!R15-Monthly_Dev!R15</f>
+        <v>8.1505277194082737E-8</v>
       </c>
       <c r="S15" s="8">
-        <f>Monthly_Op!S15-Monthly_Op!S15</f>
-        <v>0</v>
+        <f>Monthly_Op!S15-Monthly_Dev!S15</f>
+        <v>-7.2206603363156319E-8</v>
       </c>
       <c r="T15" s="8">
-        <f>Monthly_Op!T15-Monthly_Op!T15</f>
-        <v>0</v>
+        <f>Monthly_Op!T15-Monthly_Dev!T15</f>
+        <v>-4.0199665818363428E-8</v>
       </c>
       <c r="U15" s="8">
-        <f>Monthly_Op!U15-Monthly_Op!U15</f>
-        <v>0</v>
+        <f>Monthly_Op!U15-Monthly_Dev!U15</f>
+        <v>5.2359973778948188E-6</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -7381,80 +7380,80 @@
         <v>0</v>
       </c>
       <c r="C16" s="8">
-        <f>Monthly_Op!C16-Monthly_Op!C16</f>
-        <v>0</v>
+        <f>Monthly_Op!C16-Monthly_Dev!C16</f>
+        <v>-2.8403519536368549E-9</v>
       </c>
       <c r="D16" s="8">
-        <f>Monthly_Op!D16-Monthly_Op!D16</f>
-        <v>0</v>
+        <f>Monthly_Op!D16-Monthly_Dev!D16</f>
+        <v>-9.8084549000532206E-4</v>
       </c>
       <c r="E16" s="8">
-        <f>Monthly_Op!E16-Monthly_Op!E16</f>
-        <v>0</v>
+        <f>Monthly_Op!E16-Monthly_Dev!E16</f>
+        <v>-1.7210353007612866E-5</v>
       </c>
       <c r="F16" s="8">
-        <f>Monthly_Op!F16-Monthly_Op!F16</f>
+        <f>Monthly_Op!F16-Monthly_Dev!F16</f>
         <v>0</v>
       </c>
       <c r="G16" s="8">
-        <f>Monthly_Op!G16-Monthly_Op!G16</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="10">
-        <f>Monthly_Op!H16-Monthly_Op!H16</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="10">
-        <f>Monthly_Op!I16-Monthly_Op!I16</f>
-        <v>0</v>
+        <f>Monthly_Op!G16-Monthly_Dev!G16</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <f>Monthly_Op!H16-Monthly_Dev!H16</f>
+        <v>-4.8454091006533417E-4</v>
+      </c>
+      <c r="I16" s="8">
+        <f>Monthly_Op!I16-Monthly_Dev!I16</f>
+        <v>4.1039978110291031E-4</v>
       </c>
       <c r="J16" s="8">
-        <f>Monthly_Op!J16-Monthly_Op!J16</f>
-        <v>0</v>
+        <f>Monthly_Op!J16-Monthly_Dev!J16</f>
+        <v>-4.9027448767446913E-12</v>
       </c>
       <c r="K16" s="8">
-        <f>Monthly_Op!K16-Monthly_Op!K16</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="10">
-        <f>Monthly_Op!L16-Monthly_Op!L16</f>
-        <v>0</v>
+        <f>Monthly_Op!K16-Monthly_Dev!K16</f>
+        <v>5.6900262279668823E-10</v>
+      </c>
+      <c r="L16" s="8">
+        <f>Monthly_Op!L16-Monthly_Dev!L16</f>
+        <v>-4.9999751008726889E-3</v>
       </c>
       <c r="M16" s="8">
-        <f>Monthly_Op!M16-Monthly_Op!M16</f>
+        <f>Monthly_Op!M16-Monthly_Dev!M16</f>
         <v>0</v>
       </c>
       <c r="N16" s="8">
-        <f>Monthly_Op!N16-Monthly_Op!N16</f>
-        <v>0</v>
+        <f>Monthly_Op!N16-Monthly_Dev!N16</f>
+        <v>5.2300492825452238E-9</v>
       </c>
       <c r="O16" s="8">
-        <f>Monthly_Op!O16-Monthly_Op!O16</f>
-        <v>0</v>
+        <f>Monthly_Op!O16-Monthly_Dev!O16</f>
+        <v>-2.0008883439004421E-11</v>
       </c>
       <c r="P16" s="8">
-        <f>Monthly_Op!P16-Monthly_Op!P16</f>
-        <v>0</v>
+        <f>Monthly_Op!P16-Monthly_Dev!P16</f>
+        <v>-1.324006007052958E-7</v>
       </c>
       <c r="Q16" s="8">
-        <f>Monthly_Op!Q16-Monthly_Op!Q16</f>
-        <v>0</v>
+        <f>Monthly_Op!Q16-Monthly_Dev!Q16</f>
+        <v>5.314941518008709E-6</v>
       </c>
       <c r="R16" s="8">
-        <f>Monthly_Op!R16-Monthly_Op!R16</f>
-        <v>0</v>
+        <f>Monthly_Op!R16-Monthly_Dev!R16</f>
+        <v>5.7974830269813538E-8</v>
       </c>
       <c r="S16" s="8">
-        <f>Monthly_Op!S16-Monthly_Op!S16</f>
-        <v>0</v>
+        <f>Monthly_Op!S16-Monthly_Dev!S16</f>
+        <v>9.7097654361277819E-8</v>
       </c>
       <c r="T16" s="8">
-        <f>Monthly_Op!T16-Monthly_Op!T16</f>
-        <v>0</v>
+        <f>Monthly_Op!T16-Monthly_Dev!T16</f>
+        <v>-5.1899405661970377E-8</v>
       </c>
       <c r="U16" s="8">
-        <f>Monthly_Op!U16-Monthly_Op!U16</f>
-        <v>0</v>
+        <f>Monthly_Op!U16-Monthly_Dev!U16</f>
+        <v>5.1690003601834178E-6</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -7465,80 +7464,80 @@
         <v>46</v>
       </c>
       <c r="C17" s="8">
-        <f>Monthly_Op!C17-Monthly_Op!C17</f>
-        <v>0</v>
+        <f>Monthly_Op!C17-Monthly_Dev!C17</f>
+        <v>-4.9021764425560832E-10</v>
       </c>
       <c r="D17" s="8">
-        <f>Monthly_Op!D17-Monthly_Op!D17</f>
-        <v>0</v>
+        <f>Monthly_Op!D17-Monthly_Dev!D17</f>
+        <v>-1.0086419939625557E-3</v>
       </c>
       <c r="E17" s="8">
-        <f>Monthly_Op!E17-Monthly_Op!E17</f>
-        <v>0</v>
+        <f>Monthly_Op!E17-Monthly_Dev!E17</f>
+        <v>-1.725378604078287E-5</v>
       </c>
       <c r="F17" s="8">
-        <f>Monthly_Op!F17-Monthly_Op!F17</f>
+        <f>Monthly_Op!F17-Monthly_Dev!F17</f>
         <v>0</v>
       </c>
       <c r="G17" s="8">
-        <f>Monthly_Op!G17-Monthly_Op!G17</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="10">
-        <f>Monthly_Op!H17-Monthly_Op!H17</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="10">
-        <f>Monthly_Op!I17-Monthly_Op!I17</f>
-        <v>0</v>
+        <f>Monthly_Op!G17-Monthly_Dev!G17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
+        <f>Monthly_Op!H17-Monthly_Dev!H17</f>
+        <v>-4.8391114000878588E-4</v>
+      </c>
+      <c r="I17" s="8">
+        <f>Monthly_Op!I17-Monthly_Dev!I17</f>
+        <v>4.1039977649859338E-4</v>
       </c>
       <c r="J17" s="8">
-        <f>Monthly_Op!J17-Monthly_Op!J17</f>
-        <v>0</v>
+        <f>Monthly_Op!J17-Monthly_Dev!J17</f>
+        <v>-1.8587797967484221E-11</v>
       </c>
       <c r="K17" s="8">
-        <f>Monthly_Op!K17-Monthly_Op!K17</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="10">
-        <f>Monthly_Op!L17-Monthly_Op!L17</f>
-        <v>0</v>
+        <f>Monthly_Op!K17-Monthly_Dev!K17</f>
+        <v>2.6199131752946414E-10</v>
+      </c>
+      <c r="L17" s="8">
+        <f>Monthly_Op!L17-Monthly_Dev!L17</f>
+        <v>-5.0000330011243932E-3</v>
       </c>
       <c r="M17" s="8">
-        <f>Monthly_Op!M17-Monthly_Op!M17</f>
+        <f>Monthly_Op!M17-Monthly_Dev!M17</f>
         <v>0</v>
       </c>
       <c r="N17" s="8">
-        <f>Monthly_Op!N17-Monthly_Op!N17</f>
-        <v>0</v>
+        <f>Monthly_Op!N17-Monthly_Dev!N17</f>
+        <v>1.3789758668281138E-8</v>
       </c>
       <c r="O17" s="8">
-        <f>Monthly_Op!O17-Monthly_Op!O17</f>
-        <v>0</v>
+        <f>Monthly_Op!O17-Monthly_Dev!O17</f>
+        <v>-2.7400801627663895E-9</v>
       </c>
       <c r="P17" s="8">
-        <f>Monthly_Op!P17-Monthly_Op!P17</f>
-        <v>0</v>
+        <f>Monthly_Op!P17-Monthly_Dev!P17</f>
+        <v>-1.3489989214576781E-7</v>
       </c>
       <c r="Q17" s="8">
-        <f>Monthly_Op!Q17-Monthly_Op!Q17</f>
-        <v>0</v>
+        <f>Monthly_Op!Q17-Monthly_Dev!Q17</f>
+        <v>-8.1903999671339989E-7</v>
       </c>
       <c r="R17" s="8">
-        <f>Monthly_Op!R17-Monthly_Op!R17</f>
-        <v>0</v>
+        <f>Monthly_Op!R17-Monthly_Dev!R17</f>
+        <v>-6.8976078182458878E-8</v>
       </c>
       <c r="S17" s="8">
-        <f>Monthly_Op!S17-Monthly_Op!S17</f>
-        <v>0</v>
+        <f>Monthly_Op!S17-Monthly_Dev!S17</f>
+        <v>-2.1973391994833946E-9</v>
       </c>
       <c r="T17" s="8">
-        <f>Monthly_Op!T17-Monthly_Op!T17</f>
-        <v>0</v>
+        <f>Monthly_Op!T17-Monthly_Dev!T17</f>
+        <v>2.5102053768932819E-8</v>
       </c>
       <c r="U17" s="8">
-        <f>Monthly_Op!U17-Monthly_Op!U17</f>
-        <v>0</v>
+        <f>Monthly_Op!U17-Monthly_Dev!U17</f>
+        <v>1.7329875845462084E-7</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -7549,80 +7548,80 @@
         <v>47</v>
       </c>
       <c r="C18" s="8">
-        <f>Monthly_Op!C18-Monthly_Op!C18</f>
-        <v>0</v>
+        <f>Monthly_Op!C18-Monthly_Dev!C18</f>
+        <v>1.4006218407303095E-10</v>
       </c>
       <c r="D18" s="8">
-        <f>Monthly_Op!D18-Monthly_Op!D18</f>
-        <v>0</v>
+        <f>Monthly_Op!D18-Monthly_Dev!D18</f>
+        <v>-1.0196201899930202E-3</v>
       </c>
       <c r="E18" s="8">
-        <f>Monthly_Op!E18-Monthly_Op!E18</f>
-        <v>0</v>
+        <f>Monthly_Op!E18-Monthly_Dev!E18</f>
+        <v>-1.7312010982095671E-5</v>
       </c>
       <c r="F18" s="8">
-        <f>Monthly_Op!F18-Monthly_Op!F18</f>
+        <f>Monthly_Op!F18-Monthly_Dev!F18</f>
         <v>0</v>
       </c>
       <c r="G18" s="8">
-        <f>Monthly_Op!G18-Monthly_Op!G18</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="10">
-        <f>Monthly_Op!H18-Monthly_Op!H18</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="10">
-        <f>Monthly_Op!I18-Monthly_Op!I18</f>
-        <v>0</v>
+        <f>Monthly_Op!G18-Monthly_Dev!G18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="8">
+        <f>Monthly_Op!H18-Monthly_Dev!H18</f>
+        <v>-4.8349819007853512E-4</v>
+      </c>
+      <c r="I18" s="8">
+        <f>Monthly_Op!I18-Monthly_Dev!I18</f>
+        <v>4.1039974599499374E-4</v>
       </c>
       <c r="J18" s="8">
-        <f>Monthly_Op!J18-Monthly_Op!J18</f>
-        <v>0</v>
+        <f>Monthly_Op!J18-Monthly_Dev!J18</f>
+        <v>-2.0605739337042905E-11</v>
       </c>
       <c r="K18" s="8">
-        <f>Monthly_Op!K18-Monthly_Op!K18</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="10">
-        <f>Monthly_Op!L18-Monthly_Op!L18</f>
-        <v>0</v>
+        <f>Monthly_Op!K18-Monthly_Dev!K18</f>
+        <v>-8.3599616118590347E-10</v>
+      </c>
+      <c r="L18" s="8">
+        <f>Monthly_Op!L18-Monthly_Dev!L18</f>
+        <v>-5.0000070004898589E-3</v>
       </c>
       <c r="M18" s="8">
-        <f>Monthly_Op!M18-Monthly_Op!M18</f>
+        <f>Monthly_Op!M18-Monthly_Dev!M18</f>
         <v>0</v>
       </c>
       <c r="N18" s="8">
-        <f>Monthly_Op!N18-Monthly_Op!N18</f>
-        <v>0</v>
+        <f>Monthly_Op!N18-Monthly_Dev!N18</f>
+        <v>3.7002791941631585E-9</v>
       </c>
       <c r="O18" s="8">
-        <f>Monthly_Op!O18-Monthly_Op!O18</f>
-        <v>0</v>
+        <f>Monthly_Op!O18-Monthly_Dev!O18</f>
+        <v>-2.2200765670277178E-9</v>
       </c>
       <c r="P18" s="8">
-        <f>Monthly_Op!P18-Monthly_Op!P18</f>
-        <v>0</v>
+        <f>Monthly_Op!P18-Monthly_Dev!P18</f>
+        <v>-1.5859950508456677E-7</v>
       </c>
       <c r="Q18" s="8">
-        <f>Monthly_Op!Q18-Monthly_Op!Q18</f>
-        <v>0</v>
+        <f>Monthly_Op!Q18-Monthly_Dev!Q18</f>
+        <v>4.9519585445523262E-6</v>
       </c>
       <c r="R18" s="8">
-        <f>Monthly_Op!R18-Monthly_Op!R18</f>
-        <v>0</v>
+        <f>Monthly_Op!R18-Monthly_Dev!R18</f>
+        <v>-5.1019014790654182E-8</v>
       </c>
       <c r="S18" s="8">
-        <f>Monthly_Op!S18-Monthly_Op!S18</f>
-        <v>0</v>
+        <f>Monthly_Op!S18-Monthly_Dev!S18</f>
+        <v>-5.6199496611952782E-8</v>
       </c>
       <c r="T18" s="8">
-        <f>Monthly_Op!T18-Monthly_Op!T18</f>
-        <v>0</v>
+        <f>Monthly_Op!T18-Monthly_Dev!T18</f>
+        <v>4.1000021155923605E-9</v>
       </c>
       <c r="U18" s="8">
-        <f>Monthly_Op!U18-Monthly_Op!U18</f>
-        <v>0</v>
+        <f>Monthly_Op!U18-Monthly_Dev!U18</f>
+        <v>5.0280068535357714E-6</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -7633,80 +7632,80 @@
         <v>1</v>
       </c>
       <c r="C19" s="8">
-        <f>Monthly_Op!C19-Monthly_Op!C19</f>
-        <v>0</v>
+        <f>Monthly_Op!C19-Monthly_Dev!C19</f>
+        <v>3.200057108188048E-9</v>
       </c>
       <c r="D19" s="8">
-        <f>Monthly_Op!D19-Monthly_Op!D19</f>
-        <v>0</v>
+        <f>Monthly_Op!D19-Monthly_Dev!D19</f>
+        <v>-3.8571565798406482E-4</v>
       </c>
       <c r="E19" s="8">
-        <f>Monthly_Op!E19-Monthly_Op!E19</f>
-        <v>0</v>
+        <f>Monthly_Op!E19-Monthly_Dev!E19</f>
+        <v>-1.7352330019093642E-5</v>
       </c>
       <c r="F19" s="8">
-        <f>Monthly_Op!F19-Monthly_Op!F19</f>
+        <f>Monthly_Op!F19-Monthly_Dev!F19</f>
         <v>0</v>
       </c>
       <c r="G19" s="8">
-        <f>Monthly_Op!G19-Monthly_Op!G19</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="10">
-        <f>Monthly_Op!H19-Monthly_Op!H19</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="10">
-        <f>Monthly_Op!I19-Monthly_Op!I19</f>
-        <v>0</v>
+        <f>Monthly_Op!G19-Monthly_Dev!G19</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="8">
+        <f>Monthly_Op!H19-Monthly_Dev!H19</f>
+        <v>-4.8322437010028807E-4</v>
+      </c>
+      <c r="I19" s="8">
+        <f>Monthly_Op!I19-Monthly_Dev!I19</f>
+        <v>4.1039976600387718E-4</v>
       </c>
       <c r="J19" s="8">
-        <f>Monthly_Op!J19-Monthly_Op!J19</f>
-        <v>0</v>
+        <f>Monthly_Op!J19-Monthly_Dev!J19</f>
+        <v>2.1884716261411086E-12</v>
       </c>
       <c r="K19" s="8">
-        <f>Monthly_Op!K19-Monthly_Op!K19</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="10">
-        <f>Monthly_Op!L19-Monthly_Op!L19</f>
-        <v>0</v>
+        <f>Monthly_Op!K19-Monthly_Dev!K19</f>
+        <v>9.5201357908081263E-10</v>
+      </c>
+      <c r="L19" s="8">
+        <f>Monthly_Op!L19-Monthly_Dev!L19</f>
+        <v>-5.0000151004496729E-3</v>
       </c>
       <c r="M19" s="8">
-        <f>Monthly_Op!M19-Monthly_Op!M19</f>
+        <f>Monthly_Op!M19-Monthly_Dev!M19</f>
         <v>0</v>
       </c>
       <c r="N19" s="8">
-        <f>Monthly_Op!N19-Monthly_Op!N19</f>
-        <v>0</v>
+        <f>Monthly_Op!N19-Monthly_Dev!N19</f>
+        <v>-1.0869825928239152E-8</v>
       </c>
       <c r="O19" s="8">
-        <f>Monthly_Op!O19-Monthly_Op!O19</f>
-        <v>0</v>
+        <f>Monthly_Op!O19-Monthly_Dev!O19</f>
+        <v>-2.2801032173447311E-9</v>
       </c>
       <c r="P19" s="8">
-        <f>Monthly_Op!P19-Monthly_Op!P19</f>
-        <v>0</v>
+        <f>Monthly_Op!P19-Monthly_Dev!P19</f>
+        <v>-1.2669988791458309E-7</v>
       </c>
       <c r="Q19" s="8">
-        <f>Monthly_Op!Q19-Monthly_Op!Q19</f>
-        <v>0</v>
+        <f>Monthly_Op!Q19-Monthly_Dev!Q19</f>
+        <v>1.1569936759769917E-6</v>
       </c>
       <c r="R19" s="8">
-        <f>Monthly_Op!R19-Monthly_Op!R19</f>
-        <v>0</v>
+        <f>Monthly_Op!R19-Monthly_Dev!R19</f>
+        <v>4.109460860490799E-8</v>
       </c>
       <c r="S19" s="8">
-        <f>Monthly_Op!S19-Monthly_Op!S19</f>
-        <v>0</v>
+        <f>Monthly_Op!S19-Monthly_Dev!S19</f>
+        <v>-7.1697286330163479E-8</v>
       </c>
       <c r="T19" s="8">
-        <f>Monthly_Op!T19-Monthly_Op!T19</f>
-        <v>0</v>
+        <f>Monthly_Op!T19-Monthly_Dev!T19</f>
+        <v>2.0008883439004421E-9</v>
       </c>
       <c r="U19" s="8">
-        <f>Monthly_Op!U19-Monthly_Op!U19</f>
-        <v>0</v>
+        <f>Monthly_Op!U19-Monthly_Dev!U19</f>
+        <v>2.5899498723447323E-7</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -7717,80 +7716,80 @@
         <v>44</v>
       </c>
       <c r="C20" s="8">
-        <f>Monthly_Op!C20-Monthly_Op!C20</f>
-        <v>0</v>
+        <f>Monthly_Op!C20-Monthly_Dev!C20</f>
+        <v>-1.9499566406011581E-9</v>
       </c>
       <c r="D20" s="8">
-        <f>Monthly_Op!D20-Monthly_Op!D20</f>
-        <v>0</v>
+        <f>Monthly_Op!D20-Monthly_Dev!D20</f>
+        <v>2.4104439998495764E-4</v>
       </c>
       <c r="E20" s="8">
-        <f>Monthly_Op!E20-Monthly_Op!E20</f>
-        <v>0</v>
+        <f>Monthly_Op!E20-Monthly_Dev!E20</f>
+        <v>-1.7364598988933722E-5</v>
       </c>
       <c r="F20" s="8">
-        <f>Monthly_Op!F20-Monthly_Op!F20</f>
+        <f>Monthly_Op!F20-Monthly_Dev!F20</f>
         <v>0</v>
       </c>
       <c r="G20" s="8">
-        <f>Monthly_Op!G20-Monthly_Op!G20</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="10">
-        <f>Monthly_Op!H20-Monthly_Op!H20</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="10">
-        <f>Monthly_Op!I20-Monthly_Op!I20</f>
-        <v>0</v>
+        <f>Monthly_Op!G20-Monthly_Dev!G20</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="8">
+        <f>Monthly_Op!H20-Monthly_Dev!H20</f>
+        <v>-4.8304415008715296E-4</v>
+      </c>
+      <c r="I20" s="8">
+        <f>Monthly_Op!I20-Monthly_Dev!I20</f>
+        <v>4.103997785023239E-4</v>
       </c>
       <c r="J20" s="8">
-        <f>Monthly_Op!J20-Monthly_Op!J20</f>
-        <v>0</v>
+        <f>Monthly_Op!J20-Monthly_Dev!J20</f>
+        <v>-1.1098677532572765E-11</v>
       </c>
       <c r="K20" s="8">
-        <f>Monthly_Op!K20-Monthly_Op!K20</f>
-        <v>0</v>
-      </c>
-      <c r="L20" s="10">
-        <f>Monthly_Op!L20-Monthly_Op!L20</f>
-        <v>0</v>
+        <f>Monthly_Op!K20-Monthly_Dev!K20</f>
+        <v>-3.5015546018257737E-11</v>
+      </c>
+      <c r="L20" s="8">
+        <f>Monthly_Op!L20-Monthly_Dev!L20</f>
+        <v>-5.0000182691292139E-3</v>
       </c>
       <c r="M20" s="8">
-        <f>Monthly_Op!M20-Monthly_Op!M20</f>
+        <f>Monthly_Op!M20-Monthly_Dev!M20</f>
         <v>0</v>
       </c>
       <c r="N20" s="8">
-        <f>Monthly_Op!N20-Monthly_Op!N20</f>
-        <v>0</v>
+        <f>Monthly_Op!N20-Monthly_Dev!N20</f>
+        <v>1.1020347301382571E-8</v>
       </c>
       <c r="O20" s="8">
-        <f>Monthly_Op!O20-Monthly_Op!O20</f>
-        <v>0</v>
+        <f>Monthly_Op!O20-Monthly_Dev!O20</f>
+        <v>-2.7500846044858918E-9</v>
       </c>
       <c r="P20" s="8">
-        <f>Monthly_Op!P20-Monthly_Op!P20</f>
-        <v>0</v>
+        <f>Monthly_Op!P20-Monthly_Dev!P20</f>
+        <v>-1.4920078683644533E-7</v>
       </c>
       <c r="Q20" s="8">
-        <f>Monthly_Op!Q20-Monthly_Op!Q20</f>
-        <v>0</v>
+        <f>Monthly_Op!Q20-Monthly_Dev!Q20</f>
+        <v>-3.7790159694850445E-6</v>
       </c>
       <c r="R20" s="8">
-        <f>Monthly_Op!R20-Monthly_Op!R20</f>
-        <v>0</v>
+        <f>Monthly_Op!R20-Monthly_Dev!R20</f>
+        <v>7.2104739956557751E-8</v>
       </c>
       <c r="S20" s="8">
-        <f>Monthly_Op!S20-Monthly_Op!S20</f>
-        <v>0</v>
+        <f>Monthly_Op!S20-Monthly_Dev!S20</f>
+        <v>-1.0379881132394075E-7</v>
       </c>
       <c r="T20" s="8">
-        <f>Monthly_Op!T20-Monthly_Op!T20</f>
-        <v>0</v>
+        <f>Monthly_Op!T20-Monthly_Dev!T20</f>
+        <v>2.9995135264471173E-9</v>
       </c>
       <c r="U20" s="8">
-        <f>Monthly_Op!U20-Monthly_Op!U20</f>
-        <v>0</v>
+        <f>Monthly_Op!U20-Monthly_Dev!U20</f>
+        <v>-4.560992238111794E-6</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -7801,80 +7800,80 @@
         <v>44</v>
       </c>
       <c r="C21" s="8">
-        <f>Monthly_Op!C21-Monthly_Op!C21</f>
-        <v>0</v>
+        <f>Monthly_Op!C21-Monthly_Dev!C21</f>
+        <v>-2.6498128136154264E-9</v>
       </c>
       <c r="D21" s="8">
-        <f>Monthly_Op!D21-Monthly_Op!D21</f>
-        <v>0</v>
+        <f>Monthly_Op!D21-Monthly_Dev!D21</f>
+        <v>2.3643979599796694E-4</v>
       </c>
       <c r="E21" s="8">
-        <f>Monthly_Op!E21-Monthly_Op!E21</f>
-        <v>0</v>
+        <f>Monthly_Op!E21-Monthly_Dev!E21</f>
+        <v>-1.7358583022542007E-5</v>
       </c>
       <c r="F21" s="8">
-        <f>Monthly_Op!F21-Monthly_Op!F21</f>
+        <f>Monthly_Op!F21-Monthly_Dev!F21</f>
         <v>0</v>
       </c>
       <c r="G21" s="8">
-        <f>Monthly_Op!G21-Monthly_Op!G21</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="10">
-        <f>Monthly_Op!H21-Monthly_Op!H21</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="10">
-        <f>Monthly_Op!I21-Monthly_Op!I21</f>
-        <v>0</v>
+        <f>Monthly_Op!G21-Monthly_Dev!G21</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="8">
+        <f>Monthly_Op!H21-Monthly_Dev!H21</f>
+        <v>-4.8276156007887039E-4</v>
+      </c>
+      <c r="I21" s="8">
+        <f>Monthly_Op!I21-Monthly_Dev!I21</f>
+        <v>4.1039977259771376E-4</v>
       </c>
       <c r="J21" s="8">
-        <f>Monthly_Op!J21-Monthly_Op!J21</f>
-        <v>0</v>
+        <f>Monthly_Op!J21-Monthly_Dev!J21</f>
+        <v>6.1888272284704726E-11</v>
       </c>
       <c r="K21" s="8">
-        <f>Monthly_Op!K21-Monthly_Op!K21</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="10">
-        <f>Monthly_Op!L21-Monthly_Op!L21</f>
-        <v>0</v>
+        <f>Monthly_Op!K21-Monthly_Dev!K21</f>
+        <v>-7.503331289626658E-11</v>
+      </c>
+      <c r="L21" s="8">
+        <f>Monthly_Op!L21-Monthly_Dev!L21</f>
+        <v>-4.9999720013147453E-3</v>
       </c>
       <c r="M21" s="8">
-        <f>Monthly_Op!M21-Monthly_Op!M21</f>
+        <f>Monthly_Op!M21-Monthly_Dev!M21</f>
         <v>0</v>
       </c>
       <c r="N21" s="8">
-        <f>Monthly_Op!N21-Monthly_Op!N21</f>
-        <v>0</v>
+        <f>Monthly_Op!N21-Monthly_Dev!N21</f>
+        <v>-6.0699676396325231E-9</v>
       </c>
       <c r="O21" s="8">
-        <f>Monthly_Op!O21-Monthly_Op!O21</f>
-        <v>0</v>
+        <f>Monthly_Op!O21-Monthly_Dev!O21</f>
+        <v>-8.2991391536779702E-10</v>
       </c>
       <c r="P21" s="8">
-        <f>Monthly_Op!P21-Monthly_Op!P21</f>
-        <v>0</v>
+        <f>Monthly_Op!P21-Monthly_Dev!P21</f>
+        <v>-1.001990312943235E-7</v>
       </c>
       <c r="Q21" s="8">
-        <f>Monthly_Op!Q21-Monthly_Op!Q21</f>
-        <v>0</v>
+        <f>Monthly_Op!Q21-Monthly_Dev!Q21</f>
+        <v>1.2739910744130611E-6</v>
       </c>
       <c r="R21" s="8">
-        <f>Monthly_Op!R21-Monthly_Op!R21</f>
-        <v>0</v>
+        <f>Monthly_Op!R21-Monthly_Dev!R21</f>
+        <v>5.080073606222868E-8</v>
       </c>
       <c r="S21" s="8">
-        <f>Monthly_Op!S21-Monthly_Op!S21</f>
-        <v>0</v>
+        <f>Monthly_Op!S21-Monthly_Dev!S21</f>
+        <v>-4.2018655221909285E-9</v>
       </c>
       <c r="T21" s="8">
-        <f>Monthly_Op!T21-Monthly_Op!T21</f>
-        <v>0</v>
+        <f>Monthly_Op!T21-Monthly_Dev!T21</f>
+        <v>1.2005330063402653E-9</v>
       </c>
       <c r="U21" s="8">
-        <f>Monthly_Op!U21-Monthly_Op!U21</f>
-        <v>0</v>
+        <f>Monthly_Op!U21-Monthly_Dev!U21</f>
+        <v>3.3702235668897629E-7</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -7885,80 +7884,80 @@
         <v>0</v>
       </c>
       <c r="C22" s="8">
-        <f>Monthly_Op!C22-Monthly_Op!C22</f>
-        <v>0</v>
+        <f>Monthly_Op!C22-Monthly_Dev!C22</f>
+        <v>1.6007106751203537E-10</v>
       </c>
       <c r="D22" s="8">
-        <f>Monthly_Op!D22-Monthly_Op!D22</f>
-        <v>0</v>
+        <f>Monthly_Op!D22-Monthly_Dev!D22</f>
+        <v>2.3228683899390035E-4</v>
       </c>
       <c r="E22" s="8">
-        <f>Monthly_Op!E22-Monthly_Op!E22</f>
-        <v>0</v>
+        <f>Monthly_Op!E22-Monthly_Dev!E22</f>
+        <v>-1.7332304992123682E-5</v>
       </c>
       <c r="F22" s="8">
-        <f>Monthly_Op!F22-Monthly_Op!F22</f>
+        <f>Monthly_Op!F22-Monthly_Dev!F22</f>
         <v>0</v>
       </c>
       <c r="G22" s="8">
-        <f>Monthly_Op!G22-Monthly_Op!G22</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="10">
-        <f>Monthly_Op!H22-Monthly_Op!H22</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="10">
-        <f>Monthly_Op!I22-Monthly_Op!I22</f>
-        <v>0</v>
+        <f>Monthly_Op!G22-Monthly_Dev!G22</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
+        <f>Monthly_Op!H22-Monthly_Dev!H22</f>
+        <v>-4.8228916011794354E-4</v>
+      </c>
+      <c r="I22" s="8">
+        <f>Monthly_Op!I22-Monthly_Dev!I22</f>
+        <v>4.1039980190049619E-4</v>
       </c>
       <c r="J22" s="8">
-        <f>Monthly_Op!J22-Monthly_Op!J22</f>
-        <v>0</v>
+        <f>Monthly_Op!J22-Monthly_Dev!J22</f>
+        <v>-1.674038685450796E-10</v>
       </c>
       <c r="K22" s="8">
-        <f>Monthly_Op!K22-Monthly_Op!K22</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="10">
-        <f>Monthly_Op!L22-Monthly_Op!L22</f>
-        <v>0</v>
+        <f>Monthly_Op!K22-Monthly_Dev!K22</f>
+        <v>7.3907813202822581E-10</v>
+      </c>
+      <c r="L22" s="8">
+        <f>Monthly_Op!L22-Monthly_Dev!L22</f>
+        <v>-5.0000320788967656E-3</v>
       </c>
       <c r="M22" s="8">
-        <f>Monthly_Op!M22-Monthly_Op!M22</f>
+        <f>Monthly_Op!M22-Monthly_Dev!M22</f>
         <v>0</v>
       </c>
       <c r="N22" s="8">
-        <f>Monthly_Op!N22-Monthly_Op!N22</f>
-        <v>0</v>
+        <f>Monthly_Op!N22-Monthly_Dev!N22</f>
+        <v>-9.7497832030057907E-9</v>
       </c>
       <c r="O22" s="8">
-        <f>Monthly_Op!O22-Monthly_Op!O22</f>
-        <v>0</v>
+        <f>Monthly_Op!O22-Monthly_Dev!O22</f>
+        <v>-4.4997250370215625E-10</v>
       </c>
       <c r="P22" s="8">
-        <f>Monthly_Op!P22-Monthly_Op!P22</f>
-        <v>0</v>
+        <f>Monthly_Op!P22-Monthly_Dev!P22</f>
+        <v>-9.7599695436656475E-8</v>
       </c>
       <c r="Q22" s="8">
-        <f>Monthly_Op!Q22-Monthly_Op!Q22</f>
-        <v>0</v>
+        <f>Monthly_Op!Q22-Monthly_Dev!Q22</f>
+        <v>1.3369135558605194E-6</v>
       </c>
       <c r="R22" s="8">
-        <f>Monthly_Op!R22-Monthly_Op!R22</f>
-        <v>0</v>
+        <f>Monthly_Op!R22-Monthly_Dev!R22</f>
+        <v>2.5000190362334251E-8</v>
       </c>
       <c r="S22" s="8">
-        <f>Monthly_Op!S22-Monthly_Op!S22</f>
-        <v>0</v>
+        <f>Monthly_Op!S22-Monthly_Dev!S22</f>
+        <v>2.3006577976047993E-8</v>
       </c>
       <c r="T22" s="8">
-        <f>Monthly_Op!T22-Monthly_Op!T22</f>
-        <v>0</v>
+        <f>Monthly_Op!T22-Monthly_Dev!T22</f>
+        <v>-4.3000909499824047E-9</v>
       </c>
       <c r="U22" s="8">
-        <f>Monthly_Op!U22-Monthly_Op!U22</f>
-        <v>0</v>
+        <f>Monthly_Op!U22-Monthly_Dev!U22</f>
+        <v>5.4002157412469387E-7</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -7969,80 +7968,80 @@
         <v>2</v>
       </c>
       <c r="C23" s="8">
-        <f>Monthly_Op!C23-Monthly_Op!C23</f>
-        <v>0</v>
+        <f>Monthly_Op!C23-Monthly_Dev!C23</f>
+        <v>-1.3005774235352874E-10</v>
       </c>
       <c r="D23" s="8">
-        <f>Monthly_Op!D23-Monthly_Op!D23</f>
-        <v>0</v>
+        <f>Monthly_Op!D23-Monthly_Dev!D23</f>
+        <v>2.3215926300679257E-4</v>
       </c>
       <c r="E23" s="8">
-        <f>Monthly_Op!E23-Monthly_Op!E23</f>
-        <v>0</v>
+        <f>Monthly_Op!E23-Monthly_Dev!E23</f>
+        <v>-1.7289343986703898E-5</v>
       </c>
       <c r="F23" s="8">
-        <f>Monthly_Op!F23-Monthly_Op!F23</f>
+        <f>Monthly_Op!F23-Monthly_Dev!F23</f>
         <v>0</v>
       </c>
       <c r="G23" s="8">
-        <f>Monthly_Op!G23-Monthly_Op!G23</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="10">
-        <f>Monthly_Op!H23-Monthly_Op!H23</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="10">
-        <f>Monthly_Op!I23-Monthly_Op!I23</f>
-        <v>0</v>
+        <f>Monthly_Op!G23-Monthly_Dev!G23</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="8">
+        <f>Monthly_Op!H23-Monthly_Dev!H23</f>
+        <v>-4.8163457995542558E-4</v>
+      </c>
+      <c r="I23" s="8">
+        <f>Monthly_Op!I23-Monthly_Dev!I23</f>
+        <v>4.1039976860091087E-4</v>
       </c>
       <c r="J23" s="8">
-        <f>Monthly_Op!J23-Monthly_Op!J23</f>
-        <v>0</v>
+        <f>Monthly_Op!J23-Monthly_Dev!J23</f>
+        <v>1.5300827271857997E-10</v>
       </c>
       <c r="K23" s="8">
-        <f>Monthly_Op!K23-Monthly_Op!K23</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="10">
-        <f>Monthly_Op!L23-Monthly_Op!L23</f>
-        <v>0</v>
+        <f>Monthly_Op!K23-Monthly_Dev!K23</f>
+        <v>-1.0460325938765891E-9</v>
+      </c>
+      <c r="L23" s="8">
+        <f>Monthly_Op!L23-Monthly_Dev!L23</f>
+        <v>-5.000033081159927E-3</v>
       </c>
       <c r="M23" s="8">
-        <f>Monthly_Op!M23-Monthly_Op!M23</f>
+        <f>Monthly_Op!M23-Monthly_Dev!M23</f>
         <v>0</v>
       </c>
       <c r="N23" s="8">
-        <f>Monthly_Op!N23-Monthly_Op!N23</f>
-        <v>0</v>
+        <f>Monthly_Op!N23-Monthly_Dev!N23</f>
+        <v>-4.220055416226387E-9</v>
       </c>
       <c r="O23" s="8">
-        <f>Monthly_Op!O23-Monthly_Op!O23</f>
-        <v>0</v>
+        <f>Monthly_Op!O23-Monthly_Dev!O23</f>
+        <v>-2.5800090952543542E-9</v>
       </c>
       <c r="P23" s="8">
-        <f>Monthly_Op!P23-Monthly_Op!P23</f>
-        <v>0</v>
+        <f>Monthly_Op!P23-Monthly_Dev!P23</f>
+        <v>-2.1120104065630585E-7</v>
       </c>
       <c r="Q23" s="8">
-        <f>Monthly_Op!Q23-Monthly_Op!Q23</f>
-        <v>0</v>
+        <f>Monthly_Op!Q23-Monthly_Dev!Q23</f>
+        <v>9.1120018623769283E-5</v>
       </c>
       <c r="R23" s="8">
-        <f>Monthly_Op!R23-Monthly_Op!R23</f>
-        <v>0</v>
+        <f>Monthly_Op!R23-Monthly_Dev!R23</f>
+        <v>9.5984432846307755E-8</v>
       </c>
       <c r="S23" s="8">
-        <f>Monthly_Op!S23-Monthly_Op!S23</f>
-        <v>0</v>
+        <f>Monthly_Op!S23-Monthly_Dev!S23</f>
+        <v>-7.8696757555007935E-8</v>
       </c>
       <c r="T23" s="8">
-        <f>Monthly_Op!T23-Monthly_Op!T23</f>
-        <v>0</v>
+        <f>Monthly_Op!T23-Monthly_Dev!T23</f>
+        <v>6.6800566855818033E-8</v>
       </c>
       <c r="U23" s="8">
-        <f>Monthly_Op!U23-Monthly_Op!U23</f>
-        <v>0</v>
+        <f>Monthly_Op!U23-Monthly_Dev!U23</f>
+        <v>4.900200292468071E-5</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -8053,80 +8052,80 @@
         <v>47</v>
       </c>
       <c r="C24" s="8">
-        <f>Monthly_Op!C24-Monthly_Op!C24</f>
-        <v>0</v>
+        <f>Monthly_Op!C24-Monthly_Dev!C24</f>
+        <v>1.6702870198059827E-9</v>
       </c>
       <c r="D24" s="8">
-        <f>Monthly_Op!D24-Monthly_Op!D24</f>
-        <v>0</v>
+        <f>Monthly_Op!D24-Monthly_Dev!D24</f>
+        <v>5.6288132199711072E-4</v>
       </c>
       <c r="E24" s="8">
-        <f>Monthly_Op!E24-Monthly_Op!E24</f>
-        <v>0</v>
+        <f>Monthly_Op!E24-Monthly_Dev!E24</f>
+        <v>-1.7409268025403435E-5</v>
       </c>
       <c r="F24" s="8">
-        <f>Monthly_Op!F24-Monthly_Op!F24</f>
+        <f>Monthly_Op!F24-Monthly_Dev!F24</f>
         <v>0</v>
       </c>
       <c r="G24" s="8">
-        <f>Monthly_Op!G24-Monthly_Op!G24</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="10">
-        <f>Monthly_Op!H24-Monthly_Op!H24</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="10">
-        <f>Monthly_Op!I24-Monthly_Op!I24</f>
-        <v>0</v>
+        <f>Monthly_Op!G24-Monthly_Dev!G24</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="8">
+        <f>Monthly_Op!H24-Monthly_Dev!H24</f>
+        <v>-4.8005492999436683E-4</v>
+      </c>
+      <c r="I24" s="8">
+        <f>Monthly_Op!I24-Monthly_Dev!I24</f>
+        <v>4.1039978609802574E-4</v>
       </c>
       <c r="J24" s="8">
-        <f>Monthly_Op!J24-Monthly_Op!J24</f>
-        <v>0</v>
+        <f>Monthly_Op!J24-Monthly_Dev!J24</f>
+        <v>2.9199043183325557E-10</v>
       </c>
       <c r="K24" s="8">
-        <f>Monthly_Op!K24-Monthly_Op!K24</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="10">
-        <f>Monthly_Op!L24-Monthly_Op!L24</f>
-        <v>0</v>
+        <f>Monthly_Op!K24-Monthly_Dev!K24</f>
+        <v>4.2018655221909285E-10</v>
+      </c>
+      <c r="L24" s="8">
+        <f>Monthly_Op!L24-Monthly_Dev!L24</f>
+        <v>-5.0000035989796743E-3</v>
       </c>
       <c r="M24" s="8">
-        <f>Monthly_Op!M24-Monthly_Op!M24</f>
+        <f>Monthly_Op!M24-Monthly_Dev!M24</f>
         <v>0</v>
       </c>
       <c r="N24" s="8">
-        <f>Monthly_Op!N24-Monthly_Op!N24</f>
-        <v>0</v>
+        <f>Monthly_Op!N24-Monthly_Dev!N24</f>
+        <v>-5.5797499953769147E-9</v>
       </c>
       <c r="O24" s="8">
-        <f>Monthly_Op!O24-Monthly_Op!O24</f>
-        <v>0</v>
+        <f>Monthly_Op!O24-Monthly_Dev!O24</f>
+        <v>-1.3101271179039031E-9</v>
       </c>
       <c r="P24" s="8">
-        <f>Monthly_Op!P24-Monthly_Op!P24</f>
-        <v>0</v>
+        <f>Monthly_Op!P24-Monthly_Dev!P24</f>
+        <v>-2.453998604323715E-7</v>
       </c>
       <c r="Q24" s="8">
-        <f>Monthly_Op!Q24-Monthly_Op!Q24</f>
-        <v>0</v>
+        <f>Monthly_Op!Q24-Monthly_Dev!Q24</f>
+        <v>9.0539688244462013E-6</v>
       </c>
       <c r="R24" s="8">
-        <f>Monthly_Op!R24-Monthly_Op!R24</f>
-        <v>0</v>
+        <f>Monthly_Op!R24-Monthly_Dev!R24</f>
+        <v>-7.2002876549959183E-8</v>
       </c>
       <c r="S24" s="8">
-        <f>Monthly_Op!S24-Monthly_Op!S24</f>
-        <v>0</v>
+        <f>Monthly_Op!S24-Monthly_Dev!S24</f>
+        <v>7.3006958700716496E-8</v>
       </c>
       <c r="T24" s="8">
-        <f>Monthly_Op!T24-Monthly_Op!T24</f>
-        <v>0</v>
+        <f>Monthly_Op!T24-Monthly_Dev!T24</f>
+        <v>-1.9397702999413013E-8</v>
       </c>
       <c r="U24" s="8">
-        <f>Monthly_Op!U24-Monthly_Op!U24</f>
-        <v>0</v>
+        <f>Monthly_Op!U24-Monthly_Dev!U24</f>
+        <v>3.8699363358318806E-7</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -8137,80 +8136,80 @@
         <v>0</v>
       </c>
       <c r="C25" s="8">
-        <f>Monthly_Op!C25-Monthly_Op!C25</f>
-        <v>0</v>
+        <f>Monthly_Op!C25-Monthly_Dev!C25</f>
+        <v>3.3601281757000834E-9</v>
       </c>
       <c r="D25" s="8">
-        <f>Monthly_Op!D25-Monthly_Op!D25</f>
-        <v>0</v>
+        <f>Monthly_Op!D25-Monthly_Dev!D25</f>
+        <v>8.8021029603169154E-4</v>
       </c>
       <c r="E25" s="8">
-        <f>Monthly_Op!E25-Monthly_Op!E25</f>
-        <v>0</v>
+        <f>Monthly_Op!E25-Monthly_Dev!E25</f>
+        <v>-1.7441405020690581E-5</v>
       </c>
       <c r="F25" s="8">
-        <f>Monthly_Op!F25-Monthly_Op!F25</f>
+        <f>Monthly_Op!F25-Monthly_Dev!F25</f>
         <v>0</v>
       </c>
       <c r="G25" s="8">
-        <f>Monthly_Op!G25-Monthly_Op!G25</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="10">
-        <f>Monthly_Op!H25-Monthly_Op!H25</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="10">
-        <f>Monthly_Op!I25-Monthly_Op!I25</f>
-        <v>0</v>
+        <f>Monthly_Op!G25-Monthly_Dev!G25</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="8">
+        <f>Monthly_Op!H25-Monthly_Dev!H25</f>
+        <v>-4.7863875010989432E-4</v>
+      </c>
+      <c r="I25" s="8">
+        <f>Monthly_Op!I25-Monthly_Dev!I25</f>
+        <v>4.1039975990031508E-4</v>
       </c>
       <c r="J25" s="8">
-        <f>Monthly_Op!J25-Monthly_Op!J25</f>
-        <v>0</v>
+        <f>Monthly_Op!J25-Monthly_Dev!J25</f>
+        <v>2.5499957700958475E-10</v>
       </c>
       <c r="K25" s="8">
-        <f>Monthly_Op!K25-Monthly_Op!K25</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="10">
-        <f>Monthly_Op!L25-Monthly_Op!L25</f>
-        <v>0</v>
+        <f>Monthly_Op!K25-Monthly_Dev!K25</f>
+        <v>1.540229277452454E-9</v>
+      </c>
+      <c r="L25" s="8">
+        <f>Monthly_Op!L25-Monthly_Dev!L25</f>
+        <v>-4.9999902003037278E-3</v>
       </c>
       <c r="M25" s="8">
-        <f>Monthly_Op!M25-Monthly_Op!M25</f>
+        <f>Monthly_Op!M25-Monthly_Dev!M25</f>
         <v>0</v>
       </c>
       <c r="N25" s="8">
-        <f>Monthly_Op!N25-Monthly_Op!N25</f>
-        <v>0</v>
+        <f>Monthly_Op!N25-Monthly_Dev!N25</f>
+        <v>9.9498720373958349E-9</v>
       </c>
       <c r="O25" s="8">
-        <f>Monthly_Op!O25-Monthly_Op!O25</f>
-        <v>0</v>
+        <f>Monthly_Op!O25-Monthly_Dev!O25</f>
+        <v>-6.1004357121419162E-10</v>
       </c>
       <c r="P25" s="8">
-        <f>Monthly_Op!P25-Monthly_Op!P25</f>
-        <v>0</v>
+        <f>Monthly_Op!P25-Monthly_Dev!P25</f>
+        <v>-1.8460013961885124E-7</v>
       </c>
       <c r="Q25" s="8">
-        <f>Monthly_Op!Q25-Monthly_Op!Q25</f>
-        <v>0</v>
+        <f>Monthly_Op!Q25-Monthly_Dev!Q25</f>
+        <v>-5.5968994274735451E-5</v>
       </c>
       <c r="R25" s="8">
-        <f>Monthly_Op!R25-Monthly_Op!R25</f>
-        <v>0</v>
+        <f>Monthly_Op!R25-Monthly_Dev!R25</f>
+        <v>-3.3105607144534588E-8</v>
       </c>
       <c r="S25" s="8">
-        <f>Monthly_Op!S25-Monthly_Op!S25</f>
-        <v>0</v>
+        <f>Monthly_Op!S25-Monthly_Dev!S25</f>
+        <v>-1.0090298019349575E-7</v>
       </c>
       <c r="T25" s="8">
-        <f>Monthly_Op!T25-Monthly_Op!T25</f>
-        <v>0</v>
+        <f>Monthly_Op!T25-Monthly_Dev!T25</f>
+        <v>7.9002347774803638E-8</v>
       </c>
       <c r="U25" s="8">
-        <f>Monthly_Op!U25-Monthly_Op!U25</f>
-        <v>0</v>
+        <f>Monthly_Op!U25-Monthly_Dev!U25</f>
+        <v>-4.4910120777785778E-6</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -8221,80 +8220,80 @@
         <v>46</v>
       </c>
       <c r="C26" s="8">
-        <f>Monthly_Op!C26-Monthly_Op!C26</f>
-        <v>0</v>
+        <f>Monthly_Op!C26-Monthly_Dev!C26</f>
+        <v>-2.7498572308104485E-9</v>
       </c>
       <c r="D26" s="8">
-        <f>Monthly_Op!D26-Monthly_Op!D26</f>
-        <v>0</v>
+        <f>Monthly_Op!D26-Monthly_Dev!D26</f>
+        <v>7.411841010025455E-4</v>
       </c>
       <c r="E26" s="8">
-        <f>Monthly_Op!E26-Monthly_Op!E26</f>
-        <v>0</v>
+        <f>Monthly_Op!E26-Monthly_Dev!E26</f>
+        <v>-1.7150909002339176E-5</v>
       </c>
       <c r="F26" s="8">
-        <f>Monthly_Op!F26-Monthly_Op!F26</f>
+        <f>Monthly_Op!F26-Monthly_Dev!F26</f>
         <v>0</v>
       </c>
       <c r="G26" s="8">
-        <f>Monthly_Op!G26-Monthly_Op!G26</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="10">
-        <f>Monthly_Op!H26-Monthly_Op!H26</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="10">
-        <f>Monthly_Op!I26-Monthly_Op!I26</f>
-        <v>0</v>
+        <f>Monthly_Op!G26-Monthly_Dev!G26</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="8">
+        <f>Monthly_Op!H26-Monthly_Dev!H26</f>
+        <v>-4.7823035015426285E-4</v>
+      </c>
+      <c r="I26" s="8">
+        <f>Monthly_Op!I26-Monthly_Dev!I26</f>
+        <v>4.1039980830248624E-4</v>
       </c>
       <c r="J26" s="8">
-        <f>Monthly_Op!J26-Monthly_Op!J26</f>
-        <v>0</v>
+        <f>Monthly_Op!J26-Monthly_Dev!J26</f>
+        <v>4.8004267227952369E-11</v>
       </c>
       <c r="K26" s="8">
-        <f>Monthly_Op!K26-Monthly_Op!K26</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="10">
-        <f>Monthly_Op!L26-Monthly_Op!L26</f>
-        <v>0</v>
+        <f>Monthly_Op!K26-Monthly_Dev!K26</f>
+        <v>5.2295945351943374E-10</v>
+      </c>
+      <c r="L26" s="8">
+        <f>Monthly_Op!L26-Monthly_Dev!L26</f>
+        <v>-5.0000332994386554E-3</v>
       </c>
       <c r="M26" s="8">
-        <f>Monthly_Op!M26-Monthly_Op!M26</f>
+        <f>Monthly_Op!M26-Monthly_Dev!M26</f>
         <v>0</v>
       </c>
       <c r="N26" s="8">
-        <f>Monthly_Op!N26-Monthly_Op!N26</f>
-        <v>0</v>
+        <f>Monthly_Op!N26-Monthly_Dev!N26</f>
+        <v>7.6202013588044792E-9</v>
       </c>
       <c r="O26" s="8">
-        <f>Monthly_Op!O26-Monthly_Op!O26</f>
-        <v>0</v>
+        <f>Monthly_Op!O26-Monthly_Dev!O26</f>
+        <v>-3.4399363357806578E-9</v>
       </c>
       <c r="P26" s="8">
-        <f>Monthly_Op!P26-Monthly_Op!P26</f>
-        <v>0</v>
+        <f>Monthly_Op!P26-Monthly_Dev!P26</f>
+        <v>-2.0890001906082034E-7</v>
       </c>
       <c r="Q26" s="8">
-        <f>Monthly_Op!Q26-Monthly_Op!Q26</f>
-        <v>0</v>
+        <f>Monthly_Op!Q26-Monthly_Dev!Q26</f>
+        <v>4.8095942474901676E-5</v>
       </c>
       <c r="R26" s="8">
-        <f>Monthly_Op!R26-Monthly_Op!R26</f>
-        <v>0</v>
+        <f>Monthly_Op!R26-Monthly_Dev!R26</f>
+        <v>2.780143404379487E-8</v>
       </c>
       <c r="S26" s="8">
-        <f>Monthly_Op!S26-Monthly_Op!S26</f>
-        <v>0</v>
+        <f>Monthly_Op!S26-Monthly_Dev!S26</f>
+        <v>8.0501195043325424E-8</v>
       </c>
       <c r="T26" s="8">
-        <f>Monthly_Op!T26-Monthly_Op!T26</f>
-        <v>0</v>
+        <f>Monthly_Op!T26-Monthly_Dev!T26</f>
+        <v>7.890048436820507E-8</v>
       </c>
       <c r="U26" s="8">
-        <f>Monthly_Op!U26-Monthly_Op!U26</f>
-        <v>0</v>
+        <f>Monthly_Op!U26-Monthly_Dev!U26</f>
+        <v>4.8996997065842152E-5</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -8305,80 +8304,80 @@
         <v>45</v>
       </c>
       <c r="C27" s="8">
-        <f>Monthly_Op!C27-Monthly_Op!C27</f>
-        <v>0</v>
+        <f>Monthly_Op!C27-Monthly_Dev!C27</f>
+        <v>3.0699993658345193E-9</v>
       </c>
       <c r="D27" s="8">
-        <f>Monthly_Op!D27-Monthly_Op!D27</f>
-        <v>0</v>
+        <f>Monthly_Op!D27-Monthly_Dev!D27</f>
+        <v>7.3823432802555544E-4</v>
       </c>
       <c r="E27" s="8">
-        <f>Monthly_Op!E27-Monthly_Op!E27</f>
-        <v>0</v>
+        <f>Monthly_Op!E27-Monthly_Dev!E27</f>
+        <v>-1.6922052964218892E-5</v>
       </c>
       <c r="F27" s="8">
-        <f>Monthly_Op!F27-Monthly_Op!F27</f>
+        <f>Monthly_Op!F27-Monthly_Dev!F27</f>
         <v>0</v>
       </c>
       <c r="G27" s="8">
-        <f>Monthly_Op!G27-Monthly_Op!G27</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="10">
-        <f>Monthly_Op!H27-Monthly_Op!H27</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="10">
-        <f>Monthly_Op!I27-Monthly_Op!I27</f>
-        <v>0</v>
+        <f>Monthly_Op!G27-Monthly_Dev!G27</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="8">
+        <f>Monthly_Op!H27-Monthly_Dev!H27</f>
+        <v>-4.7807061014282226E-4</v>
+      </c>
+      <c r="I27" s="8">
+        <f>Monthly_Op!I27-Monthly_Dev!I27</f>
+        <v>4.1039977849521847E-4</v>
       </c>
       <c r="J27" s="8">
-        <f>Monthly_Op!J27-Monthly_Op!J27</f>
-        <v>0</v>
+        <f>Monthly_Op!J27-Monthly_Dev!J27</f>
+        <v>-3.013980176547193E-10</v>
       </c>
       <c r="K27" s="8">
-        <f>Monthly_Op!K27-Monthly_Op!K27</f>
-        <v>0</v>
-      </c>
-      <c r="L27" s="10">
-        <f>Monthly_Op!L27-Monthly_Op!L27</f>
-        <v>0</v>
+        <f>Monthly_Op!K27-Monthly_Dev!K27</f>
+        <v>-1.6802914615254849E-10</v>
+      </c>
+      <c r="L27" s="8">
+        <f>Monthly_Op!L27-Monthly_Dev!L27</f>
+        <v>-4.9999972998193698E-3</v>
       </c>
       <c r="M27" s="8">
-        <f>Monthly_Op!M27-Monthly_Op!M27</f>
+        <f>Monthly_Op!M27-Monthly_Dev!M27</f>
         <v>0</v>
       </c>
       <c r="N27" s="8">
-        <f>Monthly_Op!N27-Monthly_Op!N27</f>
-        <v>0</v>
+        <f>Monthly_Op!N27-Monthly_Dev!N27</f>
+        <v>2.5502231437712908E-9</v>
       </c>
       <c r="O27" s="8">
-        <f>Monthly_Op!O27-Monthly_Op!O27</f>
-        <v>0</v>
+        <f>Monthly_Op!O27-Monthly_Dev!O27</f>
+        <v>-3.1100171327125281E-9</v>
       </c>
       <c r="P27" s="8">
-        <f>Monthly_Op!P27-Monthly_Op!P27</f>
-        <v>0</v>
+        <f>Monthly_Op!P27-Monthly_Dev!P27</f>
+        <v>-1.7029924492817372E-7</v>
       </c>
       <c r="Q27" s="8">
-        <f>Monthly_Op!Q27-Monthly_Op!Q27</f>
-        <v>0</v>
+        <f>Monthly_Op!Q27-Monthly_Dev!Q27</f>
+        <v>5.7049328461289406E-6</v>
       </c>
       <c r="R27" s="8">
-        <f>Monthly_Op!R27-Monthly_Op!R27</f>
-        <v>0</v>
+        <f>Monthly_Op!R27-Monthly_Dev!R27</f>
+        <v>2.780143404379487E-8</v>
       </c>
       <c r="S27" s="8">
-        <f>Monthly_Op!S27-Monthly_Op!S27</f>
-        <v>0</v>
+        <f>Monthly_Op!S27-Monthly_Dev!S27</f>
+        <v>8.0501195043325424E-8</v>
       </c>
       <c r="T27" s="8">
-        <f>Monthly_Op!T27-Monthly_Op!T27</f>
-        <v>0</v>
+        <f>Monthly_Op!T27-Monthly_Dev!T27</f>
+        <v>1.8997525330632925E-8</v>
       </c>
       <c r="U27" s="8">
-        <f>Monthly_Op!U27-Monthly_Op!U27</f>
-        <v>0</v>
+        <f>Monthly_Op!U27-Monthly_Dev!U27</f>
+        <v>5.2359973778948188E-6</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -8389,80 +8388,80 @@
         <v>1</v>
       </c>
       <c r="C28" s="8">
-        <f>Monthly_Op!C28-Monthly_Op!C28</f>
-        <v>0</v>
+        <f>Monthly_Op!C28-Monthly_Dev!C28</f>
+        <v>2.6498128136154264E-9</v>
       </c>
       <c r="D28" s="8">
-        <f>Monthly_Op!D28-Monthly_Op!D28</f>
-        <v>0</v>
+        <f>Monthly_Op!D28-Monthly_Dev!D28</f>
+        <v>7.3578707900878726E-4</v>
       </c>
       <c r="E28" s="8">
-        <f>Monthly_Op!E28-Monthly_Op!E28</f>
-        <v>0</v>
+        <f>Monthly_Op!E28-Monthly_Dev!E28</f>
+        <v>-1.6836664030961401E-5</v>
       </c>
       <c r="F28" s="8">
-        <f>Monthly_Op!F28-Monthly_Op!F28</f>
+        <f>Monthly_Op!F28-Monthly_Dev!F28</f>
         <v>0</v>
       </c>
       <c r="G28" s="8">
-        <f>Monthly_Op!G28-Monthly_Op!G28</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="10">
-        <f>Monthly_Op!H28-Monthly_Op!H28</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="10">
-        <f>Monthly_Op!I28-Monthly_Op!I28</f>
-        <v>0</v>
+        <f>Monthly_Op!G28-Monthly_Dev!G28</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="8">
+        <f>Monthly_Op!H28-Monthly_Dev!H28</f>
+        <v>-4.7780721979506779E-4</v>
+      </c>
+      <c r="I28" s="8">
+        <f>Monthly_Op!I28-Monthly_Dev!I28</f>
+        <v>4.1039974320256078E-4</v>
       </c>
       <c r="J28" s="8">
-        <f>Monthly_Op!J28-Monthly_Op!J28</f>
-        <v>0</v>
+        <f>Monthly_Op!J28-Monthly_Dev!J28</f>
+        <v>-1.7905676941154525E-12</v>
       </c>
       <c r="K28" s="8">
-        <f>Monthly_Op!K28-Monthly_Op!K28</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="10">
-        <f>Monthly_Op!L28-Monthly_Op!L28</f>
-        <v>0</v>
+        <f>Monthly_Op!K28-Monthly_Dev!K28</f>
+        <v>4.7793946578167379E-10</v>
+      </c>
+      <c r="L28" s="8">
+        <f>Monthly_Op!L28-Monthly_Dev!L28</f>
+        <v>-4.9999632992694387E-3</v>
       </c>
       <c r="M28" s="8">
-        <f>Monthly_Op!M28-Monthly_Op!M28</f>
+        <f>Monthly_Op!M28-Monthly_Dev!M28</f>
         <v>0</v>
       </c>
       <c r="N28" s="8">
-        <f>Monthly_Op!N28-Monthly_Op!N28</f>
-        <v>0</v>
+        <f>Monthly_Op!N28-Monthly_Dev!N28</f>
+        <v>3.3201104088220745E-9</v>
       </c>
       <c r="O28" s="8">
-        <f>Monthly_Op!O28-Monthly_Op!O28</f>
-        <v>0</v>
+        <f>Monthly_Op!O28-Monthly_Dev!O28</f>
+        <v>-3.649802238214761E-9</v>
       </c>
       <c r="P28" s="8">
-        <f>Monthly_Op!P28-Monthly_Op!P28</f>
-        <v>0</v>
+        <f>Monthly_Op!P28-Monthly_Dev!P28</f>
+        <v>-1.8480022845324129E-7</v>
       </c>
       <c r="Q28" s="8">
-        <f>Monthly_Op!Q28-Monthly_Op!Q28</f>
-        <v>0</v>
+        <f>Monthly_Op!Q28-Monthly_Dev!Q28</f>
+        <v>5.1730312407016754E-6</v>
       </c>
       <c r="R28" s="8">
-        <f>Monthly_Op!R28-Monthly_Op!R28</f>
-        <v>0</v>
+        <f>Monthly_Op!R28-Monthly_Dev!R28</f>
+        <v>-1.6996636986732483E-8</v>
       </c>
       <c r="S28" s="8">
-        <f>Monthly_Op!S28-Monthly_Op!S28</f>
-        <v>0</v>
+        <f>Monthly_Op!S28-Monthly_Dev!S28</f>
+        <v>-5.2197719924151897E-8</v>
       </c>
       <c r="T28" s="8">
-        <f>Monthly_Op!T28-Monthly_Op!T28</f>
-        <v>0</v>
+        <f>Monthly_Op!T28-Monthly_Dev!T28</f>
+        <v>4.4001353671774268E-8</v>
       </c>
       <c r="U28" s="8">
-        <f>Monthly_Op!U28-Monthly_Op!U28</f>
-        <v>0</v>
+        <f>Monthly_Op!U28-Monthly_Dev!U28</f>
+        <v>5.1690003601834178E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added excel comparison documents which were sent to Beau to make his figures
Updated the comparison of the August integrated/operations 24 MS excel comparison document. This is the file used in the august presentations, just never pushed to git
</commit_message>
<xml_diff>
--- a/RW Files/TestModelRuns/08_August Models/Aug24MS_OpVsDev_MOST.xlsx
+++ b/RW Files/TestModelRuns/08_August Models/Aug24MS_OpVsDev_MOST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apivarnik\Desktop\GIT\MTOM\RW Files\TestModelRuns\08_August Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EBE1BA-0C5F-428E-A42B-85D275BFDC92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D8AEFC-883D-4F8F-AEDD-5462C7EBF3B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="790" activeTab="8" xr2:uid="{ACA32295-86C6-4435-AED7-5BA48188675B}"/>
   </bookViews>
@@ -27264,7 +27264,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4:Q32"/>
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28837,7 +28837,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q32"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30408,10 +30408,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615FB051-7AE9-4A87-803F-04946A35F9AB}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32369,13 +32369,70 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N30" s="2"/>
+      <c r="N30" s="16">
+        <f>Monthly_Op_LC!N30-Monthly_Dev_LC!N30</f>
+        <v>5.398760549724102E-8</v>
+      </c>
+      <c r="O30" s="16">
+        <f>Monthly_Op_LC!O30-Monthly_Dev_LC!O30</f>
+        <v>8.4699422586709261E-8</v>
+      </c>
+      <c r="P30" s="16">
+        <f>Monthly_Op_LC!P30-Monthly_Dev_LC!P30</f>
+        <v>3.2301613828167319E-8</v>
+      </c>
+      <c r="Q30" s="16">
+        <f>Monthly_Op_LC!Q30-Monthly_Dev_LC!Q30</f>
+        <v>1.7329875845462084E-7</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N31" s="2"/>
+      <c r="N31" s="16">
+        <f>Monthly_Op_LC!N31-Monthly_Dev_LC!N31</f>
+        <v>-1.6007106751203537E-8</v>
+      </c>
+      <c r="O31" s="16">
+        <f>Monthly_Op_LC!O31-Monthly_Dev_LC!O31</f>
+        <v>-6.9398083724081516E-8</v>
+      </c>
+      <c r="P31" s="16">
+        <f>Monthly_Op_LC!P31-Monthly_Dev_LC!P31</f>
+        <v>9.0221874415874481E-10</v>
+      </c>
+      <c r="Q31" s="16">
+        <f>Monthly_Op_LC!Q31-Monthly_Dev_LC!Q31</f>
+        <v>5.0280068535357714E-6</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N32" s="2"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+    </row>
+    <row r="33" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+    </row>
+    <row r="34" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+    </row>
+    <row r="35" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+    </row>
+    <row r="36" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>